<commit_message>
Update Pendulum with 2019 data
</commit_message>
<xml_diff>
--- a/PendulumPredictiveness/PastAusElectionPendulums.xlsx
+++ b/PendulumPredictiveness/PastAusElectionPendulums.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Desktop\Projects\Project Nebula\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE96268C-1CCE-4AD8-93E4-263A3999AB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A8CAC2-3C08-46F0-AD88-82C5A5417823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{0FC64BC6-A0B0-48EC-A759-65D582208678}"/>
   </bookViews>
@@ -1658,8 +1658,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="J152" sqref="J152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
@@ -7118,7 +7118,7 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2375BFFD-DFD8-43EA-880B-63C987679603}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:R152"/>
+  <dimension ref="A1:R153"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7211,15 +7211,15 @@
       </c>
       <c r="K2" s="1">
         <f>ROUND($J2+($E$153-$J$153),2)</f>
-        <v>-7.3</v>
+        <v>-7</v>
       </c>
       <c r="L2" s="1">
         <f>IF($P$7="Pre-election",ROUND($K2+($P$8-$E$153),2),ROUND($C2+($P$8-$C$153),2))</f>
-        <v>-8.18</v>
+        <v>-9.7100000000000009</v>
       </c>
       <c r="M2" s="1">
         <f>_xlfn.NORM.DIST(0,$L2,3.3,TRUE)</f>
-        <v>0.99340851598604463</v>
+        <v>0.9983717327275945</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>176</v>
@@ -7230,11 +7230,11 @@
       </c>
       <c r="Q2" s="1">
         <f ca="1">COUNTIFS(OFFSET($L$2,0,0,COUNTA($A:$A)-1,1),"&lt;0",OFFSET(IF($P$7="Pre-election",$F$2,$G$2),0,0,COUNTA($A:$A)-1,1),"")</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R2" s="1">
         <f ca="1">ROUND(SUM(OFFSET($M$2,0,0,COUNTA($A:$A)-1,1))-IF($P$7="Pre-election",SUMIFS(OFFSET($M$2,0,0,COUNTA($A:$A)-1,1),OFFSET(IF($P$7="Pre-election",$F$2,$G$2),0,0,COUNTA($A:$A)-1,1),"&lt;&gt;"&amp;""),SUMIFS(OFFSET($M$2,0,0,COUNTA($A:$A)-1,1),OFFSET($G$2,0,0,COUNTA($A:$A)-1,1),"&lt;&gt;"&amp;"")),1)</f>
-        <v>65.8</v>
+        <v>70.900000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.6">
@@ -7260,15 +7260,15 @@
       </c>
       <c r="K3" s="1">
         <f>ROUND($J3+($E$153-$J$153),2)</f>
-        <v>7.41</v>
+        <v>7.71</v>
       </c>
       <c r="L3" s="1">
         <f>IF($P$7="Pre-election",ROUND($K3+($P$8-$E$153),2),ROUND($C3+($P$8-$C$153),2))</f>
-        <v>10.130000000000001</v>
+        <v>8.6</v>
       </c>
       <c r="M3" s="1">
         <f>_xlfn.NORM.DIST(0,$L3,3.3,TRUE)</f>
-        <v>1.0713802981051001E-3</v>
+        <v>4.5795126926363016E-3</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>183</v>
@@ -7279,11 +7279,11 @@
       </c>
       <c r="Q3" s="1">
         <f ca="1">COUNTIFS(OFFSET($L$2,0,0,COUNTA($A:$A)-1,1),"&gt;0",OFFSET(IF($P$7="Pre-election",$F$2,$G$2),0,0,COUNTA($A:$A)-1,1),"")</f>
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R3" s="1">
         <f ca="1">ROUND((SUM($P$2:$P$5)-SUM(OFFSET($M$2,0,0,COUNTA($A:$A)-1,1)))-IF($P$7="Pre-election",COUNTIFS(OFFSET(IF($P$7="Pre-election",$F$2,$G$2),0,0,COUNTA($A:$A)-1,1),"&lt;&gt;"&amp;"")-SUMIFS(OFFSET($M$2,0,0,COUNTA($A:$A)-1,1),OFFSET(IF($P$7="Pre-election",$F$2,$G$2),0,0,COUNTA($A:$A)-1,1),"&lt;&gt;"&amp;""),COUNTIFS(OFFSET($G$2,0,0,COUNTA($A:$A)-1,1),"&lt;&gt;"&amp;"")-SUMIFS(OFFSET($M$2,0,0,COUNTA($A:$A)-1,1),OFFSET($G$2,0,0,COUNTA($A:$A)-1,1),"&lt;&gt;"&amp;"")),1)</f>
-        <v>79.2</v>
+        <v>74.099999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.6">
@@ -7309,15 +7309,15 @@
       </c>
       <c r="K4" s="1">
         <f>ROUND($J4+($E$153-$J$153),2)</f>
-        <v>-7.36</v>
+        <v>-7.06</v>
       </c>
       <c r="L4" s="1">
         <f>IF($P$7="Pre-election",ROUND($K4+($P$8-$E$153),2),ROUND($C4+($P$8-$C$153),2))</f>
-        <v>-10.98</v>
+        <v>-12.51</v>
       </c>
       <c r="M4" s="1">
         <f>_xlfn.NORM.DIST(0,$L4,3.3,TRUE)</f>
-        <v>0.99956149752483647</v>
+        <v>0.99992495155524597</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>184</v>
@@ -7354,15 +7354,15 @@
       </c>
       <c r="K5" s="1">
         <f>ROUND($J5+($E$153-$J$153),2)</f>
-        <v>1.44</v>
+        <v>1.74</v>
       </c>
       <c r="L5" s="1">
         <f>IF($P$7="Pre-election",ROUND($K5+($P$8-$E$153),2),ROUND($C5+($P$8-$C$153),2))</f>
-        <v>6.26</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="M5" s="1">
         <f>_xlfn.NORM.DIST(0,$L5,3.3,TRUE)</f>
-        <v>2.8915968818961062E-2</v>
+        <v>7.5881300172258054E-2</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>185</v>
@@ -7399,15 +7399,15 @@
       </c>
       <c r="K6" s="1">
         <f>ROUND($J6+($E$153-$J$153),2)</f>
-        <v>13.88</v>
+        <v>14.18</v>
       </c>
       <c r="L6" s="1">
         <f>IF($P$7="Pre-election",ROUND($K6+($P$8-$E$153),2),ROUND($C6+($P$8-$C$153),2))</f>
-        <v>18.95</v>
+        <v>17.420000000000002</v>
       </c>
       <c r="M6" s="1">
         <f>_xlfn.NORM.DIST(0,$L6,3.3,TRUE)</f>
-        <v>4.6665318840292792E-9</v>
+        <v>6.5020618946445036E-8</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.6">
@@ -7439,15 +7439,15 @@
       </c>
       <c r="K7" s="1">
         <f>ROUND($J7+($E$153-$J$153),2)</f>
-        <v>-10.31</v>
+        <v>-10.01</v>
       </c>
       <c r="L7" s="1">
         <f>IF($P$7="Pre-election",ROUND($K7+($P$8-$E$153),2),ROUND($C7+($P$8-$C$153),2))</f>
-        <v>-9.42</v>
+        <v>-10.95</v>
       </c>
       <c r="M7" s="1">
         <f>_xlfn.NORM.DIST(0,$L7,3.3,TRUE)</f>
-        <v>0.99784507680908341</v>
+        <v>0.99954697257326042</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>204</v>
@@ -7485,15 +7485,15 @@
       </c>
       <c r="K8" s="1">
         <f>ROUND($J8+($E$153-$J$153),2)</f>
-        <v>-7.42</v>
+        <v>-7.12</v>
       </c>
       <c r="L8" s="1">
         <f>IF($P$7="Pre-election",ROUND($K8+($P$8-$E$153),2),ROUND($C8+($P$8-$C$153),2))</f>
-        <v>0.41</v>
+        <v>-1.1200000000000001</v>
       </c>
       <c r="M8" s="1">
         <f>_xlfn.NORM.DIST(0,$L8,3.3,TRUE)</f>
-        <v>0.45056166637593642</v>
+        <v>0.63284350819591806</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>190</v>
@@ -7525,15 +7525,15 @@
       </c>
       <c r="K9" s="1">
         <f>ROUND($J9+($E$153-$J$153),2)</f>
-        <v>-8.85</v>
+        <v>-8.5500000000000007</v>
       </c>
       <c r="L9" s="1">
         <f>IF($P$7="Pre-election",ROUND($K9+($P$8-$E$153),2),ROUND($C9+($P$8-$C$153),2))</f>
-        <v>-7.52</v>
+        <v>-9.0500000000000007</v>
       </c>
       <c r="M9" s="1">
         <f>_xlfn.NORM.DIST(0,$L9,3.3,TRUE)</f>
-        <v>0.98866016110376231</v>
+        <v>0.99695062418912472</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.6">
@@ -7559,15 +7559,15 @@
       </c>
       <c r="K10" s="1">
         <f>ROUND($J10+($E$153-$J$153),2)</f>
-        <v>-3.87</v>
+        <v>-3.57</v>
       </c>
       <c r="L10" s="1">
         <f>IF($P$7="Pre-election",ROUND($K10+($P$8-$E$153),2),ROUND($C10+($P$8-$C$153),2))</f>
-        <v>-9.0399999999999991</v>
+        <v>-10.57</v>
       </c>
       <c r="M10" s="1">
         <f>_xlfn.NORM.DIST(0,$L10,3.3,TRUE)</f>
-        <v>0.9969223714464196</v>
+        <v>0.99932005164583071</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.6">
@@ -7593,15 +7593,15 @@
       </c>
       <c r="K11" s="1">
         <f>ROUND($J11+($E$153-$J$153),2)</f>
-        <v>9.7200000000000006</v>
+        <v>10.02</v>
       </c>
       <c r="L11" s="1">
         <f>IF($P$7="Pre-election",ROUND($K11+($P$8-$E$153),2),ROUND($C11+($P$8-$C$153),2))</f>
-        <v>6.91</v>
+        <v>5.38</v>
       </c>
       <c r="M11" s="1">
         <f>_xlfn.NORM.DIST(0,$L11,3.3,TRUE)</f>
-        <v>1.8132689720230428E-2</v>
+        <v>5.1518733721893091E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.6">
@@ -7627,15 +7627,15 @@
       </c>
       <c r="K12" s="1">
         <f>ROUND($J12+($E$153-$J$153),2)</f>
-        <v>16.45</v>
+        <v>16.75</v>
       </c>
       <c r="L12" s="1">
         <f>IF($P$7="Pre-election",ROUND($K12+($P$8-$E$153),2),ROUND($C12+($P$8-$C$153),2))</f>
-        <v>15.65</v>
+        <v>14.12</v>
       </c>
       <c r="M12" s="1">
         <f>_xlfn.NORM.DIST(0,$L12,3.3,TRUE)</f>
-        <v>1.0558790470129999E-6</v>
+        <v>9.3956918450265829E-6</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.6">
@@ -7661,15 +7661,15 @@
       </c>
       <c r="K13" s="1">
         <f>ROUND($J13+($E$153-$J$153),2)</f>
-        <v>-8.14</v>
+        <v>-7.84</v>
       </c>
       <c r="L13" s="1">
         <f>IF($P$7="Pre-election",ROUND($K13+($P$8-$E$153),2),ROUND($C13+($P$8-$C$153),2))</f>
-        <v>-1.21</v>
+        <v>-2.74</v>
       </c>
       <c r="M13" s="1">
         <f>_xlfn.NORM.DIST(0,$L13,3.3,TRUE)</f>
-        <v>0.64306616326250143</v>
+        <v>0.79681626239306391</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.6">
@@ -7695,15 +7695,15 @@
       </c>
       <c r="K14" s="1">
         <f>ROUND($J14+($E$153-$J$153),2)</f>
-        <v>-19.48</v>
+        <v>-19.18</v>
       </c>
       <c r="L14" s="1">
         <f>IF($P$7="Pre-election",ROUND($K14+($P$8-$E$153),2),ROUND($C14+($P$8-$C$153),2))</f>
-        <v>-14.72</v>
+        <v>-16.25</v>
       </c>
       <c r="M14" s="1">
         <f>_xlfn.NORM.DIST(0,$L14,3.3,TRUE)</f>
-        <v>0.99999591359001394</v>
+        <v>0.99999957656101846</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.6">
@@ -7729,15 +7729,15 @@
       </c>
       <c r="K15" s="1">
         <f>ROUND($J15+($E$153-$J$153),2)</f>
-        <v>3.39</v>
+        <v>3.69</v>
       </c>
       <c r="L15" s="1">
         <f>IF($P$7="Pre-election",ROUND($K15+($P$8-$E$153),2),ROUND($C15+($P$8-$C$153),2))</f>
-        <v>7.41</v>
+        <v>5.88</v>
       </c>
       <c r="M15" s="1">
         <f>_xlfn.NORM.DIST(0,$L15,3.3,TRUE)</f>
-        <v>1.2369483570798966E-2</v>
+        <v>3.7389443145740137E-2</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.6">
@@ -7763,15 +7763,15 @@
       </c>
       <c r="K16" s="1">
         <f>ROUND($J16+($E$153-$J$153),2)</f>
-        <v>2.71</v>
+        <v>3.01</v>
       </c>
       <c r="L16" s="1">
         <f>IF($P$7="Pre-election",ROUND($K16+($P$8-$E$153),2),ROUND($C16+($P$8-$C$153),2))</f>
-        <v>1.38</v>
+        <v>-0.15</v>
       </c>
       <c r="M16" s="1">
         <f>_xlfn.NORM.DIST(0,$L16,3.3,TRUE)</f>
-        <v>0.3379070940676977</v>
+        <v>0.51812749755218657</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.6">
@@ -7797,15 +7797,15 @@
       </c>
       <c r="K17" s="1">
         <f>ROUND($J17+($E$153-$J$153),2)</f>
-        <v>7.07</v>
+        <v>7.37</v>
       </c>
       <c r="L17" s="1">
         <f>IF($P$7="Pre-election",ROUND($K17+($P$8-$E$153),2),ROUND($C17+($P$8-$C$153),2))</f>
-        <v>10.24</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="M17" s="1">
         <f>_xlfn.NORM.DIST(0,$L17,3.3,TRUE)</f>
-        <v>9.5775012874509157E-4</v>
+        <v>4.1527203404563631E-3</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.6">
@@ -7837,15 +7837,15 @@
       </c>
       <c r="K18" s="1">
         <f>ROUND($J18+($E$153-$J$153),2)</f>
-        <v>-3.73</v>
+        <v>-3.43</v>
       </c>
       <c r="L18" s="1">
         <f>IF($P$7="Pre-election",ROUND($K18+($P$8-$E$153),2),ROUND($C18+($P$8-$C$153),2))</f>
-        <v>3.09</v>
+        <v>1.56</v>
       </c>
       <c r="M18" s="1">
         <f>_xlfn.NORM.DIST(0,$L18,3.3,TRUE)</f>
-        <v>0.1745429969217818</v>
+        <v>0.31820388324170745</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.6">
@@ -7871,15 +7871,15 @@
       </c>
       <c r="K19" s="1">
         <f>ROUND($J19+($E$153-$J$153),2)</f>
-        <v>21.04</v>
+        <v>21.34</v>
       </c>
       <c r="L19" s="1">
         <f>IF($P$7="Pre-election",ROUND($K19+($P$8-$E$153),2),ROUND($C19+($P$8-$C$153),2))</f>
-        <v>16.559999999999999</v>
+        <v>15.03</v>
       </c>
       <c r="M19" s="1">
         <f>_xlfn.NORM.DIST(0,$L19,3.3,TRUE)</f>
-        <v>2.6081399100878626E-7</v>
+        <v>2.6249486240520106E-6</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.6">
@@ -7905,15 +7905,15 @@
       </c>
       <c r="K20" s="1">
         <f>ROUND($J20+($E$153-$J$153),2)</f>
-        <v>-11.43</v>
+        <v>-11.13</v>
       </c>
       <c r="L20" s="1">
         <f>IF($P$7="Pre-election",ROUND($K20+($P$8-$E$153),2),ROUND($C20+($P$8-$C$153),2))</f>
-        <v>-6.66</v>
+        <v>-8.19</v>
       </c>
       <c r="M20" s="1">
         <f>_xlfn.NORM.DIST(0,$L20,3.3,TRUE)</f>
-        <v>0.9782138354957719</v>
+        <v>0.99346430236754257</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.6">
@@ -7939,15 +7939,15 @@
       </c>
       <c r="K21" s="1">
         <f>ROUND($J21+($E$153-$J$153),2)</f>
-        <v>6</v>
+        <v>6.3</v>
       </c>
       <c r="L21" s="1">
         <f>IF($P$7="Pre-election",ROUND($K21+($P$8-$E$153),2),ROUND($C21+($P$8-$C$153),2))</f>
-        <v>4.92</v>
+        <v>3.39</v>
       </c>
       <c r="M21" s="1">
         <f>_xlfn.NORM.DIST(0,$L21,3.3,TRUE)</f>
-        <v>6.7992682137644297E-2</v>
+        <v>0.15214603037208185</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.6">
@@ -7973,15 +7973,15 @@
       </c>
       <c r="K22" s="1">
         <f>ROUND($J22+($E$153-$J$153),2)</f>
-        <v>-14.05</v>
+        <v>-13.75</v>
       </c>
       <c r="L22" s="1">
         <f>IF($P$7="Pre-election",ROUND($K22+($P$8-$E$153),2),ROUND($C22+($P$8-$C$153),2))</f>
-        <v>-14.15</v>
+        <v>-15.68</v>
       </c>
       <c r="M22" s="1">
         <f>_xlfn.NORM.DIST(0,$L22,3.3,TRUE)</f>
-        <v>0.99999098062612446</v>
+        <v>0.99999899050986363</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.6">
@@ -8007,15 +8007,15 @@
       </c>
       <c r="K23" s="1">
         <f>ROUND($J23+($E$153-$J$153),2)</f>
-        <v>-7.11</v>
+        <v>-6.81</v>
       </c>
       <c r="L23" s="1">
         <f>IF($P$7="Pre-election",ROUND($K23+($P$8-$E$153),2),ROUND($C23+($P$8-$C$153),2))</f>
-        <v>-4.99</v>
+        <v>-6.52</v>
       </c>
       <c r="M23" s="1">
         <f>_xlfn.NORM.DIST(0,$L23,3.3,TRUE)</f>
-        <v>0.93474848525336485</v>
+        <v>0.97590887976440399</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.6">
@@ -8041,15 +8041,15 @@
       </c>
       <c r="K24" s="1">
         <f>ROUND($J24+($E$153-$J$153),2)</f>
-        <v>11.81</v>
+        <v>12.11</v>
       </c>
       <c r="L24" s="1">
         <f>IF($P$7="Pre-election",ROUND($K24+($P$8-$E$153),2),ROUND($C24+($P$8-$C$153),2))</f>
-        <v>13.29</v>
+        <v>11.76</v>
       </c>
       <c r="M24" s="1">
         <f>_xlfn.NORM.DIST(0,$L24,3.3,TRUE)</f>
-        <v>2.8213783550347004E-5</v>
+        <v>1.828762756389531E-4</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.6">
@@ -8075,15 +8075,15 @@
       </c>
       <c r="K25" s="1">
         <f>ROUND($J25+($E$153-$J$153),2)</f>
-        <v>-19.73</v>
+        <v>-19.43</v>
       </c>
       <c r="L25" s="1">
         <f>IF($P$7="Pre-election",ROUND($K25+($P$8-$E$153),2),ROUND($C25+($P$8-$C$153),2))</f>
-        <v>-18.8</v>
+        <v>-20.329999999999998</v>
       </c>
       <c r="M25" s="1">
         <f>_xlfn.NORM.DIST(0,$L25,3.3,TRUE)</f>
-        <v>0.99999999390222027</v>
+        <v>0.99999999963766473</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.6">
@@ -8112,15 +8112,15 @@
       </c>
       <c r="K26" s="1">
         <f>ROUND($J26+($E$153-$J$153),2)</f>
-        <v>-11.94</v>
+        <v>-11.64</v>
       </c>
       <c r="L26" s="1">
         <f>IF($P$7="Pre-election",ROUND($K26+($P$8-$E$153),2),ROUND($C26+($P$8-$C$153),2))</f>
-        <v>-17.079999999999998</v>
+        <v>-18.61</v>
       </c>
       <c r="M26" s="1">
         <f>_xlfn.NORM.DIST(0,$L26,3.3,TRUE)</f>
-        <v>0.99999988650598248</v>
+        <v>0.99999999146751384</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.6">
@@ -8146,15 +8146,15 @@
       </c>
       <c r="K27" s="1">
         <f>ROUND($J27+($E$153-$J$153),2)</f>
-        <v>6.79</v>
+        <v>7.09</v>
       </c>
       <c r="L27" s="1">
         <f>IF($P$7="Pre-election",ROUND($K27+($P$8-$E$153),2),ROUND($C27+($P$8-$C$153),2))</f>
-        <v>11.55</v>
+        <v>10.02</v>
       </c>
       <c r="M27" s="1">
         <f>_xlfn.NORM.DIST(0,$L27,3.3,TRUE)</f>
-        <v>2.3262907903552461E-4</v>
+        <v>1.1972519568347209E-3</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.6">
@@ -8180,15 +8180,15 @@
       </c>
       <c r="K28" s="1">
         <f>ROUND($J28+($E$153-$J$153),2)</f>
-        <v>0.64</v>
+        <v>0.94</v>
       </c>
       <c r="L28" s="1">
         <f>IF($P$7="Pre-election",ROUND($K28+($P$8-$E$153),2),ROUND($C28+($P$8-$C$153),2))</f>
-        <v>12.36</v>
+        <v>10.83</v>
       </c>
       <c r="M28" s="1">
         <f>_xlfn.NORM.DIST(0,$L28,3.3,TRUE)</f>
-        <v>9.0033724640428741E-5</v>
+        <v>5.1570043260429149E-4</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.6">
@@ -8214,15 +8214,15 @@
       </c>
       <c r="K29" s="1">
         <f>ROUND($J29+($E$153-$J$153),2)</f>
-        <v>4.55</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="L29" s="1">
         <f>IF($P$7="Pre-election",ROUND($K29+($P$8-$E$153),2),ROUND($C29+($P$8-$C$153),2))</f>
-        <v>4.6500000000000004</v>
+        <v>3.12</v>
       </c>
       <c r="M29" s="1">
         <f>_xlfn.NORM.DIST(0,$L29,3.3,TRUE)</f>
-        <v>7.9404144314309713E-2</v>
+        <v>0.17221343315296905</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.6">
@@ -8248,15 +8248,15 @@
       </c>
       <c r="K30" s="1">
         <f>ROUND($J30+($E$153-$J$153),2)</f>
-        <v>-19.190000000000001</v>
+        <v>-18.89</v>
       </c>
       <c r="L30" s="1">
         <f>IF($P$7="Pre-election",ROUND($K30+($P$8-$E$153),2),ROUND($C30+($P$8-$C$153),2))</f>
-        <v>-12.37</v>
+        <v>-13.9</v>
       </c>
       <c r="M30" s="1">
         <f>_xlfn.NORM.DIST(0,$L30,3.3,TRUE)</f>
-        <v>0.99991104695852795</v>
+        <v>0.99998735081400791</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.6">
@@ -8285,15 +8285,15 @@
       </c>
       <c r="K31" s="1">
         <f>ROUND($J31+($E$153-$J$153),2)</f>
-        <v>3.91</v>
+        <v>4.21</v>
       </c>
       <c r="L31" s="1">
         <f>IF($P$7="Pre-election",ROUND($K31+($P$8-$E$153),2),ROUND($C31+($P$8-$C$153),2))</f>
-        <v>0.56999999999999995</v>
+        <v>-0.96</v>
       </c>
       <c r="M31" s="1">
         <f>_xlfn.NORM.DIST(0,$L31,3.3,TRUE)</f>
-        <v>0.43143290272648549</v>
+        <v>0.6144395758352782</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.6">
@@ -8325,15 +8325,15 @@
       </c>
       <c r="K32" s="1">
         <f>ROUND($J32+($E$153-$J$153),2)</f>
-        <v>-15.34</v>
+        <v>-15.04</v>
       </c>
       <c r="L32" s="1">
         <f>IF($P$7="Pre-election",ROUND($K32+($P$8-$E$153),2),ROUND($C32+($P$8-$C$153),2))</f>
-        <v>-16.18</v>
+        <v>-17.71</v>
       </c>
       <c r="M32" s="1">
         <f>_xlfn.NORM.DIST(0,$L32,3.3,TRUE)</f>
-        <v>0.99999952815290194</v>
+        <v>0.99999995989745682</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.6">
@@ -8359,15 +8359,15 @@
       </c>
       <c r="K33" s="1">
         <f>ROUND($J33+($E$153-$J$153),2)</f>
-        <v>15.39</v>
+        <v>15.69</v>
       </c>
       <c r="L33" s="1">
         <f>IF($P$7="Pre-election",ROUND($K33+($P$8-$E$153),2),ROUND($C33+($P$8-$C$153),2))</f>
-        <v>19.02</v>
+        <v>17.489999999999998</v>
       </c>
       <c r="M33" s="1">
         <f>_xlfn.NORM.DIST(0,$L33,3.3,TRUE)</f>
-        <v>4.1160341051471963E-9</v>
+        <v>5.7901340399645781E-8</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.6">
@@ -8393,15 +8393,15 @@
       </c>
       <c r="K34" s="1">
         <f>ROUND($J34+($E$153-$J$153),2)</f>
-        <v>-22.1</v>
+        <v>-21.8</v>
       </c>
       <c r="L34" s="1">
         <f>IF($P$7="Pre-election",ROUND($K34+($P$8-$E$153),2),ROUND($C34+($P$8-$C$153),2))</f>
-        <v>-26.33</v>
+        <v>-27.86</v>
       </c>
       <c r="M34" s="1">
         <f>_xlfn.NORM.DIST(0,$L34,3.3,TRUE)</f>
-        <v>0.99999999999999922</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.6">
@@ -8427,15 +8427,15 @@
       </c>
       <c r="K35" s="1">
         <f>ROUND($J35+($E$153-$J$153),2)</f>
-        <v>-0.03</v>
+        <v>0.27</v>
       </c>
       <c r="L35" s="1">
         <f>IF($P$7="Pre-election",ROUND($K35+($P$8-$E$153),2),ROUND($C35+($P$8-$C$153),2))</f>
-        <v>-1.07</v>
+        <v>-2.6</v>
       </c>
       <c r="M35" s="1">
         <f>_xlfn.NORM.DIST(0,$L35,3.3,TRUE)</f>
-        <v>0.62712274719470196</v>
+        <v>0.78461619507109481</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.6">
@@ -8461,15 +8461,15 @@
       </c>
       <c r="K36" s="1">
         <f>ROUND($J36+($E$153-$J$153),2)</f>
-        <v>-8.2100000000000009</v>
+        <v>-7.91</v>
       </c>
       <c r="L36" s="1">
         <f>IF($P$7="Pre-election",ROUND($K36+($P$8-$E$153),2),ROUND($C36+($P$8-$C$153),2))</f>
-        <v>-10.33</v>
+        <v>-11.86</v>
       </c>
       <c r="M36" s="1">
         <f>_xlfn.NORM.DIST(0,$L36,3.3,TRUE)</f>
-        <v>0.99912686968268094</v>
+        <v>0.99983714218420805</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.6">
@@ -8501,15 +8501,15 @@
       </c>
       <c r="K37" s="1">
         <f>ROUND($J37+($E$153-$J$153),2)</f>
-        <v>-2.69</v>
+        <v>-2.39</v>
       </c>
       <c r="L37" s="1">
         <f>IF($P$7="Pre-election",ROUND($K37+($P$8-$E$153),2),ROUND($C37+($P$8-$C$153),2))</f>
-        <v>-0.84</v>
+        <v>-2.37</v>
       </c>
       <c r="M37" s="1">
         <f>_xlfn.NORM.DIST(0,$L37,3.3,TRUE)</f>
-        <v>0.60046290373674682</v>
+        <v>0.76367740643658755</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.6">
@@ -8538,15 +8538,15 @@
       </c>
       <c r="K38" s="1">
         <f>ROUND($J38+($E$153-$J$153),2)</f>
-        <v>11.58</v>
+        <v>11.88</v>
       </c>
       <c r="L38" s="1">
         <f>IF($P$7="Pre-election",ROUND($K38+($P$8-$E$153),2),ROUND($C38+($P$8-$C$153),2))</f>
-        <v>11.88</v>
+        <v>10.35</v>
       </c>
       <c r="M38" s="1">
         <f>_xlfn.NORM.DIST(0,$L38,3.3,TRUE)</f>
-        <v>1.5910859015753318E-4</v>
+        <v>8.5528482121784058E-4</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.6">
@@ -8572,15 +8572,15 @@
       </c>
       <c r="K39" s="1">
         <f>ROUND($J39+($E$153-$J$153),2)</f>
-        <v>-13.32</v>
+        <v>-13.02</v>
       </c>
       <c r="L39" s="1">
         <f>IF($P$7="Pre-election",ROUND($K39+($P$8-$E$153),2),ROUND($C39+($P$8-$C$153),2))</f>
-        <v>-13.41</v>
+        <v>-14.94</v>
       </c>
       <c r="M39" s="1">
         <f>_xlfn.NORM.DIST(0,$L39,3.3,TRUE)</f>
-        <v>0.99997584296245012</v>
+        <v>0.99999701250967787</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.6">
@@ -8609,15 +8609,15 @@
       </c>
       <c r="K40" s="1">
         <f>ROUND($J40+($E$153-$J$153),2)</f>
-        <v>19.7</v>
+        <v>20</v>
       </c>
       <c r="L40" s="1">
         <f>IF($P$7="Pre-election",ROUND($K40+($P$8-$E$153),2),ROUND($C40+($P$8-$C$153),2))</f>
-        <v>14.33</v>
+        <v>12.8</v>
       </c>
       <c r="M40" s="1">
         <f>_xlfn.NORM.DIST(0,$L40,3.3,TRUE)</f>
-        <v>7.0459542170090736E-6</v>
+        <v>5.2489121683448526E-5</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.6">
@@ -8643,15 +8643,15 @@
       </c>
       <c r="K41" s="1">
         <f>ROUND($J41+($E$153-$J$153),2)</f>
-        <v>3.37</v>
+        <v>3.67</v>
       </c>
       <c r="L41" s="1">
         <f>IF($P$7="Pre-election",ROUND($K41+($P$8-$E$153),2),ROUND($C41+($P$8-$C$153),2))</f>
-        <v>14.61</v>
+        <v>13.08</v>
       </c>
       <c r="M41" s="1">
         <f>_xlfn.NORM.DIST(0,$L41,3.3,TRUE)</f>
-        <v>4.7716019539925549E-6</v>
+        <v>3.6908333213782731E-5</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.6">
@@ -8677,15 +8677,15 @@
       </c>
       <c r="K42" s="1">
         <f>ROUND($J42+($E$153-$J$153),2)</f>
-        <v>6.44</v>
+        <v>6.74</v>
       </c>
       <c r="L42" s="1">
         <f>IF($P$7="Pre-election",ROUND($K42+($P$8-$E$153),2),ROUND($C42+($P$8-$C$153),2))</f>
-        <v>4.78</v>
+        <v>3.25</v>
       </c>
       <c r="M42" s="1">
         <f>_xlfn.NORM.DIST(0,$L42,3.3,TRUE)</f>
-        <v>7.3740750196920987E-2</v>
+        <v>0.16234925038176298</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.6">
@@ -8711,15 +8711,15 @@
       </c>
       <c r="K43" s="1">
         <f>ROUND($J43+($E$153-$J$153),2)</f>
-        <v>1.69</v>
+        <v>1.99</v>
       </c>
       <c r="L43" s="1">
         <f>IF($P$7="Pre-election",ROUND($K43+($P$8-$E$153),2),ROUND($C43+($P$8-$C$153),2))</f>
-        <v>4.6399999999999997</v>
+        <v>3.11</v>
       </c>
       <c r="M43" s="1">
         <f>_xlfn.NORM.DIST(0,$L43,3.3,TRUE)</f>
-        <v>7.9853064444918825E-2</v>
+        <v>0.17298774023280908</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.6">
@@ -8751,15 +8751,15 @@
       </c>
       <c r="K44" s="1">
         <f>ROUND($J44+($E$153-$J$153),2)</f>
-        <v>-6.81</v>
+        <v>-6.51</v>
       </c>
       <c r="L44" s="1">
         <f>IF($P$7="Pre-election",ROUND($K44+($P$8-$E$153),2),ROUND($C44+($P$8-$C$153),2))</f>
-        <v>-1.5</v>
+        <v>-3.03</v>
       </c>
       <c r="M44" s="1">
         <f>_xlfn.NORM.DIST(0,$L44,3.3,TRUE)</f>
-        <v>0.67528185813662267</v>
+        <v>0.82073815709586695</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.6">
@@ -8785,15 +8785,15 @@
       </c>
       <c r="K45" s="1">
         <f>ROUND($J45+($E$153-$J$153),2)</f>
-        <v>-1.03</v>
+        <v>-0.73</v>
       </c>
       <c r="L45" s="1">
         <f>IF($P$7="Pre-election",ROUND($K45+($P$8-$E$153),2),ROUND($C45+($P$8-$C$153),2))</f>
-        <v>-2.74</v>
+        <v>-4.2699999999999996</v>
       </c>
       <c r="M45" s="1">
         <f>_xlfn.NORM.DIST(0,$L45,3.3,TRUE)</f>
-        <v>0.79681626239306391</v>
+        <v>0.90215682207138048</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.6">
@@ -8819,15 +8819,15 @@
       </c>
       <c r="K46" s="1">
         <f>ROUND($J46+($E$153-$J$153),2)</f>
-        <v>11.06</v>
+        <v>11.36</v>
       </c>
       <c r="L46" s="1">
         <f>IF($P$7="Pre-election",ROUND($K46+($P$8-$E$153),2),ROUND($C46+($P$8-$C$153),2))</f>
-        <v>14.76</v>
+        <v>13.23</v>
       </c>
       <c r="M46" s="1">
         <f>_xlfn.NORM.DIST(0,$L46,3.3,TRUE)</f>
-        <v>3.8614124465986952E-6</v>
+        <v>3.0476474713237599E-5</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.6">
@@ -8859,15 +8859,15 @@
       </c>
       <c r="K47" s="1">
         <f>ROUND($J47+($E$153-$J$153),2)</f>
-        <v>-4.93</v>
+        <v>-4.63</v>
       </c>
       <c r="L47" s="1">
         <f>IF($P$7="Pre-election",ROUND($K47+($P$8-$E$153),2),ROUND($C47+($P$8-$C$153),2))</f>
-        <v>-0.85</v>
+        <v>-2.38</v>
       </c>
       <c r="M47" s="1">
         <f>_xlfn.NORM.DIST(0,$L47,3.3,TRUE)</f>
-        <v>0.60163282940665874</v>
+        <v>0.76461049238936707</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.6">
@@ -8893,15 +8893,15 @@
       </c>
       <c r="K48" s="1">
         <f>ROUND($J48+($E$153-$J$153),2)</f>
-        <v>11.24</v>
+        <v>11.54</v>
       </c>
       <c r="L48" s="1">
         <f>IF($P$7="Pre-election",ROUND($K48+($P$8-$E$153),2),ROUND($C48+($P$8-$C$153),2))</f>
-        <v>14.18</v>
+        <v>12.65</v>
       </c>
       <c r="M48" s="1">
         <f>_xlfn.NORM.DIST(0,$L48,3.3,TRUE)</f>
-        <v>8.6574427251357542E-6</v>
+        <v>6.3209231868402554E-5</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.6">
@@ -8927,15 +8927,15 @@
       </c>
       <c r="K49" s="1">
         <f>ROUND($J49+($E$153-$J$153),2)</f>
-        <v>10.87</v>
+        <v>11.17</v>
       </c>
       <c r="L49" s="1">
         <f>IF($P$7="Pre-election",ROUND($K49+($P$8-$E$153),2),ROUND($C49+($P$8-$C$153),2))</f>
-        <v>13.44</v>
+        <v>11.91</v>
       </c>
       <c r="M49" s="1">
         <f>_xlfn.NORM.DIST(0,$L49,3.3,TRUE)</f>
-        <v>2.3232911175214924E-5</v>
+        <v>1.536359618892075E-4</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.6">
@@ -8961,15 +8961,15 @@
       </c>
       <c r="K50" s="1">
         <f>ROUND($J50+($E$153-$J$153),2)</f>
-        <v>20.53</v>
+        <v>20.83</v>
       </c>
       <c r="L50" s="1">
         <f>IF($P$7="Pre-election",ROUND($K50+($P$8-$E$153),2),ROUND($C50+($P$8-$C$153),2))</f>
-        <v>19.829999999999998</v>
+        <v>18.3</v>
       </c>
       <c r="M50" s="1">
         <f>_xlfn.NORM.DIST(0,$L50,3.3,TRUE)</f>
-        <v>9.3283247404068115E-10</v>
+        <v>1.4659574876468052E-8</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.6">
@@ -8995,15 +8995,15 @@
       </c>
       <c r="K51" s="1">
         <f>ROUND($J51+($E$153-$J$153),2)</f>
-        <v>-11.84</v>
+        <v>-11.54</v>
       </c>
       <c r="L51" s="1">
         <f>IF($P$7="Pre-election",ROUND($K51+($P$8-$E$153),2),ROUND($C51+($P$8-$C$153),2))</f>
-        <v>-10.56</v>
+        <v>-12.09</v>
       </c>
       <c r="M51" s="1">
         <f>_xlfn.NORM.DIST(0,$L51,3.3,TRUE)</f>
-        <v>0.99931286206208414</v>
+        <v>0.99987567013127621</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.6">
@@ -9029,15 +9029,15 @@
       </c>
       <c r="K52" s="1">
         <f>ROUND($J52+($E$153-$J$153),2)</f>
-        <v>9.15</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="L52" s="1">
         <f>IF($P$7="Pre-election",ROUND($K52+($P$8-$E$153),2),ROUND($C52+($P$8-$C$153),2))</f>
-        <v>12.7</v>
+        <v>11.17</v>
       </c>
       <c r="M52" s="1">
         <f>_xlfn.NORM.DIST(0,$L52,3.3,TRUE)</f>
-        <v>5.9425323241526937E-5</v>
+        <v>3.5608776942661492E-4</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.6">
@@ -9063,15 +9063,15 @@
       </c>
       <c r="K53" s="1">
         <f>ROUND($J53+($E$153-$J$153),2)</f>
-        <v>7.01</v>
+        <v>7.31</v>
       </c>
       <c r="L53" s="1">
         <f>IF($P$7="Pre-election",ROUND($K53+($P$8-$E$153),2),ROUND($C53+($P$8-$C$153),2))</f>
-        <v>5.64</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="M53" s="1">
         <f>_xlfn.NORM.DIST(0,$L53,3.3,TRUE)</f>
-        <v>4.3717055636634805E-2</v>
+        <v>0.10648235697293514</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.6">
@@ -9097,15 +9097,15 @@
       </c>
       <c r="K54" s="1">
         <f>ROUND($J54+($E$153-$J$153),2)</f>
-        <v>1.04</v>
+        <v>1.34</v>
       </c>
       <c r="L54" s="1">
         <f>IF($P$7="Pre-election",ROUND($K54+($P$8-$E$153),2),ROUND($C54+($P$8-$C$153),2))</f>
-        <v>8.66</v>
+        <v>7.13</v>
       </c>
       <c r="M54" s="1">
         <f>_xlfn.NORM.DIST(0,$L54,3.3,TRUE)</f>
-        <v>4.3420974847200164E-3</v>
+        <v>1.5362891432752546E-2</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.6">
@@ -9131,15 +9131,15 @@
       </c>
       <c r="K55" s="1">
         <f>ROUND($J55+($E$153-$J$153),2)</f>
-        <v>0.63</v>
+        <v>0.93</v>
       </c>
       <c r="L55" s="1">
         <f>IF($P$7="Pre-election",ROUND($K55+($P$8-$E$153),2),ROUND($C55+($P$8-$C$153),2))</f>
-        <v>8.6</v>
+        <v>7.07</v>
       </c>
       <c r="M55" s="1">
         <f>_xlfn.NORM.DIST(0,$L55,3.3,TRUE)</f>
-        <v>4.5795126926363016E-3</v>
+        <v>1.6079679418778619E-2</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.6">
@@ -9165,15 +9165,15 @@
       </c>
       <c r="K56" s="1">
         <f>ROUND($J56+($E$153-$J$153),2)</f>
-        <v>12.56</v>
+        <v>12.86</v>
       </c>
       <c r="L56" s="1">
         <f>IF($P$7="Pre-election",ROUND($K56+($P$8-$E$153),2),ROUND($C56+($P$8-$C$153),2))</f>
-        <v>14.56</v>
+        <v>13.03</v>
       </c>
       <c r="M56" s="1">
         <f>_xlfn.NORM.DIST(0,$L56,3.3,TRUE)</f>
-        <v>5.1181388111743097E-6</v>
+        <v>3.9323696377353822E-5</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.6">
@@ -9199,15 +9199,15 @@
       </c>
       <c r="K57" s="1">
         <f>ROUND($J57+($E$153-$J$153),2)</f>
-        <v>-17.489999999999998</v>
+        <v>-17.190000000000001</v>
       </c>
       <c r="L57" s="1">
         <f>IF($P$7="Pre-election",ROUND($K57+($P$8-$E$153),2),ROUND($C57+($P$8-$C$153),2))</f>
-        <v>-13.99</v>
+        <v>-15.52</v>
       </c>
       <c r="M57" s="1">
         <f>_xlfn.NORM.DIST(0,$L57,3.3,TRUE)</f>
-        <v>0.9999887937973807</v>
+        <v>0.99999871835821041</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.6">
@@ -9233,15 +9233,15 @@
       </c>
       <c r="K58" s="1">
         <f>ROUND($J58+($E$153-$J$153),2)</f>
-        <v>-10.73</v>
+        <v>-10.43</v>
       </c>
       <c r="L58" s="1">
         <f>IF($P$7="Pre-election",ROUND($K58+($P$8-$E$153),2),ROUND($C58+($P$8-$C$153),2))</f>
-        <v>-12.21</v>
+        <v>-13.74</v>
       </c>
       <c r="M58" s="1">
         <f>_xlfn.NORM.DIST(0,$L58,3.3,TRUE)</f>
-        <v>0.99989220026652259</v>
+        <v>0.99998433905915363</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.6">
@@ -9267,15 +9267,15 @@
       </c>
       <c r="K59" s="1">
         <f>ROUND($J59+($E$153-$J$153),2)</f>
-        <v>-19.79</v>
+        <v>-19.489999999999998</v>
       </c>
       <c r="L59" s="1">
         <f>IF($P$7="Pre-election",ROUND($K59+($P$8-$E$153),2),ROUND($C59+($P$8-$C$153),2))</f>
-        <v>-14.18</v>
+        <v>-15.71</v>
       </c>
       <c r="M59" s="1">
         <f>_xlfn.NORM.DIST(0,$L59,3.3,TRUE)</f>
-        <v>0.99999134255727484</v>
+        <v>0.99999903493765219</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.6">
@@ -9301,15 +9301,15 @@
       </c>
       <c r="K60" s="1">
         <f>ROUND($J60+($E$153-$J$153),2)</f>
-        <v>-7.52</v>
+        <v>-7.22</v>
       </c>
       <c r="L60" s="1">
         <f>IF($P$7="Pre-election",ROUND($K60+($P$8-$E$153),2),ROUND($C60+($P$8-$C$153),2))</f>
-        <v>-6.92</v>
+        <v>-8.4499999999999993</v>
       </c>
       <c r="M60" s="1">
         <f>_xlfn.NORM.DIST(0,$L60,3.3,TRUE)</f>
-        <v>0.98200187103269643</v>
+        <v>0.99477551179937429</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.6">
@@ -9335,15 +9335,15 @@
       </c>
       <c r="K61" s="1">
         <f>ROUND($J61+($E$153-$J$153),2)</f>
-        <v>-15.12</v>
+        <v>-14.82</v>
       </c>
       <c r="L61" s="1">
         <f>IF($P$7="Pre-election",ROUND($K61+($P$8-$E$153),2),ROUND($C61+($P$8-$C$153),2))</f>
-        <v>-14.83</v>
+        <v>-16.36</v>
       </c>
       <c r="M61" s="1">
         <f>_xlfn.NORM.DIST(0,$L61,3.3,TRUE)</f>
-        <v>0.9999965041232608</v>
+        <v>0.99999964310893374</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.6">
@@ -9372,15 +9372,15 @@
       </c>
       <c r="K62" s="1">
         <f>ROUND($J62+($E$153-$J$153),2)</f>
-        <v>-0.27</v>
+        <v>0.03</v>
       </c>
       <c r="L62" s="1">
         <f>IF($P$7="Pre-election",ROUND($K62+($P$8-$E$153),2),ROUND($C62+($P$8-$C$153),2))</f>
-        <v>-2.61</v>
+        <v>-4.1399999999999997</v>
       </c>
       <c r="M62" s="1">
         <f>_xlfn.NORM.DIST(0,$L62,3.3,TRUE)</f>
-        <v>0.78550147848047613</v>
+        <v>0.89517809247410773</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.6">
@@ -9406,15 +9406,15 @@
       </c>
       <c r="K63" s="1">
         <f>ROUND($J63+($E$153-$J$153),2)</f>
-        <v>18.21</v>
+        <v>18.510000000000002</v>
       </c>
       <c r="L63" s="1">
         <f>IF($P$7="Pre-election",ROUND($K63+($P$8-$E$153),2),ROUND($C63+($P$8-$C$153),2))</f>
-        <v>16.670000000000002</v>
+        <v>15.14</v>
       </c>
       <c r="M63" s="1">
         <f>_xlfn.NORM.DIST(0,$L63,3.3,TRUE)</f>
-        <v>2.1915957988420728E-7</v>
+        <v>2.2388624159193738E-6</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.6">
@@ -9440,15 +9440,15 @@
       </c>
       <c r="K64" s="1">
         <f>ROUND($J64+($E$153-$J$153),2)</f>
-        <v>12.68</v>
+        <v>12.98</v>
       </c>
       <c r="L64" s="1">
         <f>IF($P$7="Pre-election",ROUND($K64+($P$8-$E$153),2),ROUND($C64+($P$8-$C$153),2))</f>
-        <v>7.79</v>
+        <v>6.26</v>
       </c>
       <c r="M64" s="1">
         <f>_xlfn.NORM.DIST(0,$L64,3.3,TRUE)</f>
-        <v>9.1225501602054792E-3</v>
+        <v>2.8915968818961062E-2</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.6">
@@ -9474,15 +9474,15 @@
       </c>
       <c r="K65" s="1">
         <f>ROUND($J65+($E$153-$J$153),2)</f>
-        <v>-18.489999999999998</v>
+        <v>-18.190000000000001</v>
       </c>
       <c r="L65" s="1">
         <f>IF($P$7="Pre-election",ROUND($K65+($P$8-$E$153),2),ROUND($C65+($P$8-$C$153),2))</f>
-        <v>-15.36</v>
+        <v>-16.89</v>
       </c>
       <c r="M65" s="1">
         <f>_xlfn.NORM.DIST(0,$L65,3.3,TRUE)</f>
-        <v>0.99999837651897883</v>
+        <v>0.99999984575243139</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.6">
@@ -9508,15 +9508,15 @@
       </c>
       <c r="K66" s="1">
         <f>ROUND($J66+($E$153-$J$153),2)</f>
-        <v>-22.36</v>
+        <v>-22.06</v>
       </c>
       <c r="L66" s="1">
         <f>IF($P$7="Pre-election",ROUND($K66+($P$8-$E$153),2),ROUND($C66+($P$8-$C$153),2))</f>
-        <v>-23.83</v>
+        <v>-25.36</v>
       </c>
       <c r="M66" s="1">
         <f>_xlfn.NORM.DIST(0,$L66,3.3,TRUE)</f>
-        <v>0.99999999999974232</v>
+        <v>0.99999999999999234</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.6">
@@ -9542,15 +9542,15 @@
       </c>
       <c r="K67" s="1">
         <f>ROUND($J67+($E$153-$J$153),2)</f>
-        <v>-6.31</v>
+        <v>-6.01</v>
       </c>
       <c r="L67" s="1">
         <f>IF($P$7="Pre-election",ROUND($K67+($P$8-$E$153),2),ROUND($C67+($P$8-$C$153),2))</f>
-        <v>-2.8</v>
+        <v>-4.33</v>
       </c>
       <c r="M67" s="1">
         <f>_xlfn.NORM.DIST(0,$L67,3.3,TRUE)</f>
-        <v>0.80191599648040313</v>
+        <v>0.90526038004796039</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.6">
@@ -9576,15 +9576,15 @@
       </c>
       <c r="K68" s="1">
         <f>ROUND($J68+($E$153-$J$153),2)</f>
-        <v>7.75</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="L68" s="1">
         <f>IF($P$7="Pre-election",ROUND($K68+($P$8-$E$153),2),ROUND($C68+($P$8-$C$153),2))</f>
-        <v>13.32</v>
+        <v>11.79</v>
       </c>
       <c r="M68" s="1">
         <f>_xlfn.NORM.DIST(0,$L68,3.3,TRUE)</f>
-        <v>2.7143027202953619E-5</v>
+        <v>1.7664132093786104E-4</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.6">
@@ -9610,15 +9610,15 @@
       </c>
       <c r="K69" s="1">
         <f>ROUND($J69+($E$153-$J$153),2)</f>
-        <v>-1.43</v>
+        <v>-1.1299999999999999</v>
       </c>
       <c r="L69" s="1">
         <f>IF($P$7="Pre-election",ROUND($K69+($P$8-$E$153),2),ROUND($C69+($P$8-$C$153),2))</f>
-        <v>-2.86</v>
+        <v>-4.3899999999999997</v>
       </c>
       <c r="M69" s="1">
         <f>_xlfn.NORM.DIST(0,$L69,3.3,TRUE)</f>
-        <v>0.8069376628580931</v>
+        <v>0.90829077541631409</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.6">
@@ -9644,15 +9644,15 @@
       </c>
       <c r="K70" s="1">
         <f>ROUND($J70+($E$153-$J$153),2)</f>
-        <v>15.31</v>
+        <v>15.61</v>
       </c>
       <c r="L70" s="1">
         <f>IF($P$7="Pre-election",ROUND($K70+($P$8-$E$153),2),ROUND($C70+($P$8-$C$153),2))</f>
-        <v>20.48</v>
+        <v>18.95</v>
       </c>
       <c r="M70" s="1">
         <f>_xlfn.NORM.DIST(0,$L70,3.3,TRUE)</f>
-        <v>2.7164616722090893E-10</v>
+        <v>4.6665318840292792E-9</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.6">
@@ -9678,15 +9678,15 @@
       </c>
       <c r="K71" s="1">
         <f>ROUND($J71+($E$153-$J$153),2)</f>
-        <v>2.0499999999999998</v>
+        <v>2.35</v>
       </c>
       <c r="L71" s="1">
         <f>IF($P$7="Pre-election",ROUND($K71+($P$8-$E$153),2),ROUND($C71+($P$8-$C$153),2))</f>
-        <v>5.39</v>
+        <v>3.86</v>
       </c>
       <c r="M71" s="1">
         <f>_xlfn.NORM.DIST(0,$L71,3.3,TRUE)</f>
-        <v>5.1199454917107826E-2</v>
+        <v>0.12106146903118314</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.6">
@@ -9718,15 +9718,15 @@
       </c>
       <c r="K72" s="1">
         <f>ROUND($J72+($E$153-$J$153),2)</f>
-        <v>-2.02</v>
+        <v>-1.72</v>
       </c>
       <c r="L72" s="1">
         <f>IF($P$7="Pre-election",ROUND($K72+($P$8-$E$153),2),ROUND($C72+($P$8-$C$153),2))</f>
-        <v>8.36</v>
+        <v>6.83</v>
       </c>
       <c r="M72" s="1">
         <f>_xlfn.NORM.DIST(0,$L72,3.3,TRUE)</f>
-        <v>5.6491727555606384E-3</v>
+        <v>1.9240365355672685E-2</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.6">
@@ -9755,15 +9755,15 @@
       </c>
       <c r="K73" s="1">
         <f>ROUND($J73+($E$153-$J$153),2)</f>
-        <v>8.9700000000000006</v>
+        <v>9.27</v>
       </c>
       <c r="L73" s="1">
         <f>IF($P$7="Pre-election",ROUND($K73+($P$8-$E$153),2),ROUND($C73+($P$8-$C$153),2))</f>
-        <v>3.88</v>
+        <v>2.35</v>
       </c>
       <c r="M73" s="1">
         <f>_xlfn.NORM.DIST(0,$L73,3.3,TRUE)</f>
-        <v>0.11984588187261838</v>
+        <v>0.23819485997038672</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.6">
@@ -9795,15 +9795,15 @@
       </c>
       <c r="K74" s="1">
         <f>ROUND($J74+($E$153-$J$153),2)</f>
-        <v>-10.43</v>
+        <v>-10.130000000000001</v>
       </c>
       <c r="L74" s="1">
         <f>IF($P$7="Pre-election",ROUND($K74+($P$8-$E$153),2),ROUND($C74+($P$8-$C$153),2))</f>
-        <v>-6.54</v>
+        <v>-8.07</v>
       </c>
       <c r="M74" s="1">
         <f>_xlfn.NORM.DIST(0,$L74,3.3,TRUE)</f>
-        <v>0.97625020311780686</v>
+        <v>0.99276651583435538</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.6">
@@ -9829,15 +9829,15 @@
       </c>
       <c r="K75" s="1">
         <f>ROUND($J75+($E$153-$J$153),2)</f>
-        <v>8.3800000000000008</v>
+        <v>8.68</v>
       </c>
       <c r="L75" s="1">
         <f>IF($P$7="Pre-election",ROUND($K75+($P$8-$E$153),2),ROUND($C75+($P$8-$C$153),2))</f>
-        <v>14.5</v>
+        <v>12.97</v>
       </c>
       <c r="M75" s="1">
         <f>_xlfn.NORM.DIST(0,$L75,3.3,TRUE)</f>
-        <v>5.5657430455985187E-6</v>
+        <v>4.2419434935297943E-5</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.6">
@@ -9863,15 +9863,15 @@
       </c>
       <c r="K76" s="1">
         <f>ROUND($J76+($E$153-$J$153),2)</f>
-        <v>-9.94</v>
+        <v>-9.64</v>
       </c>
       <c r="L76" s="1">
         <f>IF($P$7="Pre-election",ROUND($K76+($P$8-$E$153),2),ROUND($C76+($P$8-$C$153),2))</f>
-        <v>-8.6999999999999993</v>
+        <v>-10.23</v>
       </c>
       <c r="M76" s="1">
         <f>_xlfn.NORM.DIST(0,$L76,3.3,TRUE)</f>
-        <v>0.99581000627949312</v>
+        <v>0.99903239678678168</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.6">
@@ -9897,15 +9897,15 @@
       </c>
       <c r="K77" s="1">
         <f>ROUND($J77+($E$153-$J$153),2)</f>
-        <v>-4.21</v>
+        <v>-3.91</v>
       </c>
       <c r="L77" s="1">
         <f>IF($P$7="Pre-election",ROUND($K77+($P$8-$E$153),2),ROUND($C77+($P$8-$C$153),2))</f>
-        <v>-5.91</v>
+        <v>-7.44</v>
       </c>
       <c r="M77" s="1">
         <f>_xlfn.NORM.DIST(0,$L77,3.3,TRUE)</f>
-        <v>0.96334605769516335</v>
+        <v>0.98791906275512631</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.6">
@@ -9931,15 +9931,15 @@
       </c>
       <c r="K78" s="1">
         <f>ROUND($J78+($E$153-$J$153),2)</f>
-        <v>9.33</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="L78" s="1">
         <f>IF($P$7="Pre-election",ROUND($K78+($P$8-$E$153),2),ROUND($C78+($P$8-$C$153),2))</f>
-        <v>9.85</v>
+        <v>8.32</v>
       </c>
       <c r="M78" s="1">
         <f>_xlfn.NORM.DIST(0,$L78,3.3,TRUE)</f>
-        <v>1.4185940984381463E-3</v>
+        <v>5.8475663663904894E-3</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.6">
@@ -9965,15 +9965,15 @@
       </c>
       <c r="K79" s="1">
         <f>ROUND($J79+($E$153-$J$153),2)</f>
-        <v>10.18</v>
+        <v>10.48</v>
       </c>
       <c r="L79" s="1">
         <f>IF($P$7="Pre-election",ROUND($K79+($P$8-$E$153),2),ROUND($C79+($P$8-$C$153),2))</f>
-        <v>12.99</v>
+        <v>11.46</v>
       </c>
       <c r="M79" s="1">
         <f>_xlfn.NORM.DIST(0,$L79,3.3,TRUE)</f>
-        <v>4.1362795907138388E-5</v>
+        <v>2.5759929897277098E-4</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.6">
@@ -9999,15 +9999,15 @@
       </c>
       <c r="K80" s="1">
         <f>ROUND($J80+($E$153-$J$153),2)</f>
-        <v>-12.46</v>
+        <v>-12.16</v>
       </c>
       <c r="L80" s="1">
         <f>IF($P$7="Pre-election",ROUND($K80+($P$8-$E$153),2),ROUND($C80+($P$8-$C$153),2))</f>
-        <v>-2.98</v>
+        <v>-4.51</v>
       </c>
       <c r="M80" s="1">
         <f>_xlfn.NORM.DIST(0,$L80,3.3,TRUE)</f>
-        <v>0.81674509383387672</v>
+        <v>0.91413509474264409</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.6">
@@ -10039,15 +10039,15 @@
       </c>
       <c r="K81" s="1">
         <f>ROUND($J81+($E$153-$J$153),2)</f>
-        <v>5.01</v>
+        <v>5.31</v>
       </c>
       <c r="L81" s="1">
         <f>IF($P$7="Pre-election",ROUND($K81+($P$8-$E$153),2),ROUND($C81+($P$8-$C$153),2))</f>
-        <v>12.73</v>
+        <v>11.2</v>
       </c>
       <c r="M81" s="1">
         <f>_xlfn.NORM.DIST(0,$L81,3.3,TRUE)</f>
-        <v>5.7258595494450212E-5</v>
+        <v>3.4447468841684848E-4</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.6">
@@ -10073,15 +10073,15 @@
       </c>
       <c r="K82" s="1">
         <f>ROUND($J82+($E$153-$J$153),2)</f>
-        <v>-2.98</v>
+        <v>-2.68</v>
       </c>
       <c r="L82" s="1">
         <f>IF($P$7="Pre-election",ROUND($K82+($P$8-$E$153),2),ROUND($C82+($P$8-$C$153),2))</f>
-        <v>-6.43</v>
+        <v>-7.96</v>
       </c>
       <c r="M82" s="1">
         <f>_xlfn.NORM.DIST(0,$L82,3.3,TRUE)</f>
-        <v>0.97432151198197015</v>
+        <v>0.9920699960871322</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.6">
@@ -10110,15 +10110,15 @@
       </c>
       <c r="K83" s="1">
         <f>ROUND($J83+($E$153-$J$153),2)</f>
-        <v>-4.5999999999999996</v>
+        <v>-4.3</v>
       </c>
       <c r="L83" s="1">
         <f>IF($P$7="Pre-election",ROUND($K83+($P$8-$E$153),2),ROUND($C83+($P$8-$C$153),2))</f>
-        <v>-6.57</v>
+        <v>-8.1</v>
       </c>
       <c r="M83" s="1">
         <f>_xlfn.NORM.DIST(0,$L83,3.3,TRUE)</f>
-        <v>0.97675455870747474</v>
+        <v>0.99294685852631026</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.6">
@@ -10150,15 +10150,15 @@
       </c>
       <c r="K84" s="1">
         <f>ROUND($J84+($E$153-$J$153),2)</f>
-        <v>6.74</v>
+        <v>7.04</v>
       </c>
       <c r="L84" s="1">
         <f>IF($P$7="Pre-election",ROUND($K84+($P$8-$E$153),2),ROUND($C84+($P$8-$C$153),2))</f>
-        <v>14.51</v>
+        <v>12.98</v>
       </c>
       <c r="M84" s="1">
         <f>_xlfn.NORM.DIST(0,$L84,3.3,TRUE)</f>
-        <v>5.4886331724951466E-6</v>
+        <v>4.1887966890061208E-5</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.6">
@@ -10184,15 +10184,15 @@
       </c>
       <c r="K85" s="1">
         <f>ROUND($J85+($E$153-$J$153),2)</f>
-        <v>-8.57</v>
+        <v>-8.27</v>
       </c>
       <c r="L85" s="1">
         <f>IF($P$7="Pre-election",ROUND($K85+($P$8-$E$153),2),ROUND($C85+($P$8-$C$153),2))</f>
-        <v>-8.81</v>
+        <v>-10.34</v>
       </c>
       <c r="M85" s="1">
         <f>_xlfn.NORM.DIST(0,$L85,3.3,TRUE)</f>
-        <v>0.99620401351748689</v>
+        <v>0.99913583479090196</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.6">
@@ -10218,15 +10218,15 @@
       </c>
       <c r="K86" s="1">
         <f>ROUND($J86+($E$153-$J$153),2)</f>
-        <v>-13.55</v>
+        <v>-13.25</v>
       </c>
       <c r="L86" s="1">
         <f>IF($P$7="Pre-election",ROUND($K86+($P$8-$E$153),2),ROUND($C86+($P$8-$C$153),2))</f>
-        <v>-11.94</v>
+        <v>-13.47</v>
       </c>
       <c r="M86" s="1">
         <f>_xlfn.NORM.DIST(0,$L86,3.3,TRUE)</f>
-        <v>0.99985166002475867</v>
+        <v>0.9999776576255055</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.6">
@@ -10252,15 +10252,15 @@
       </c>
       <c r="K87" s="1">
         <f>ROUND($J87+($E$153-$J$153),2)</f>
-        <v>12.82</v>
+        <v>13.12</v>
       </c>
       <c r="L87" s="1">
         <f>IF($P$7="Pre-election",ROUND($K87+($P$8-$E$153),2),ROUND($C87+($P$8-$C$153),2))</f>
-        <v>6.68</v>
+        <v>5.15</v>
       </c>
       <c r="M87" s="1">
         <f>_xlfn.NORM.DIST(0,$L87,3.3,TRUE)</f>
-        <v>2.147260722467224E-2</v>
+        <v>5.9308363958881179E-2</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.6">
@@ -10286,15 +10286,15 @@
       </c>
       <c r="K88" s="1">
         <f>ROUND($J88+($E$153-$J$153),2)</f>
-        <v>3.22</v>
+        <v>3.52</v>
       </c>
       <c r="L88" s="1">
         <f>IF($P$7="Pre-election",ROUND($K88+($P$8-$E$153),2),ROUND($C88+($P$8-$C$153),2))</f>
-        <v>4.49</v>
+        <v>2.96</v>
       </c>
       <c r="M88" s="1">
         <f>_xlfn.NORM.DIST(0,$L88,3.3,TRUE)</f>
-        <v>8.6819107649624555E-2</v>
+        <v>0.18486754357536259</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.6">
@@ -10320,15 +10320,15 @@
       </c>
       <c r="K89" s="1">
         <f>ROUND($J89+($E$153-$J$153),2)</f>
-        <v>-14.19</v>
+        <v>-13.89</v>
       </c>
       <c r="L89" s="1">
         <f>IF($P$7="Pre-election",ROUND($K89+($P$8-$E$153),2),ROUND($C89+($P$8-$C$153),2))</f>
-        <v>-12.41</v>
+        <v>-13.94</v>
       </c>
       <c r="M89" s="1">
         <f>_xlfn.NORM.DIST(0,$L89,3.3,TRUE)</f>
-        <v>0.9999152489060753</v>
+        <v>0.9999880127063292</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.6">
@@ -10354,15 +10354,15 @@
       </c>
       <c r="K90" s="1">
         <f>ROUND($J90+($E$153-$J$153),2)</f>
-        <v>3.95</v>
+        <v>4.25</v>
       </c>
       <c r="L90" s="1">
         <f>IF($P$7="Pre-election",ROUND($K90+($P$8-$E$153),2),ROUND($C90+($P$8-$C$153),2))</f>
-        <v>4.17</v>
+        <v>2.64</v>
       </c>
       <c r="M90" s="1">
         <f>_xlfn.NORM.DIST(0,$L90,3.3,TRUE)</f>
-        <v>0.10318028772671951</v>
+        <v>0.21185539858339661</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.6">
@@ -10391,15 +10391,15 @@
       </c>
       <c r="K91" s="1">
         <f>ROUND($J91+($E$153-$J$153),2)</f>
-        <v>-4.68</v>
+        <v>-4.38</v>
       </c>
       <c r="L91" s="1">
         <f>IF($P$7="Pre-election",ROUND($K91+($P$8-$E$153),2),ROUND($C91+($P$8-$C$153),2))</f>
-        <v>-0.64</v>
+        <v>-2.17</v>
       </c>
       <c r="M91" s="1">
         <f>_xlfn.NORM.DIST(0,$L91,3.3,TRUE)</f>
-        <v>0.57688833132229345</v>
+        <v>0.74459461183263898</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.6">
@@ -10428,15 +10428,15 @@
       </c>
       <c r="K92" s="1">
         <f>ROUND($J92+($E$153-$J$153),2)</f>
-        <v>-0.11</v>
+        <v>0.19</v>
       </c>
       <c r="L92" s="1">
         <f>IF($P$7="Pre-election",ROUND($K92+($P$8-$E$153),2),ROUND($C92+($P$8-$C$153),2))</f>
-        <v>5.04</v>
+        <v>3.51</v>
       </c>
       <c r="M92" s="1">
         <f>_xlfn.NORM.DIST(0,$L92,3.3,TRUE)</f>
-        <v>6.3346604125778819E-2</v>
+        <v>0.14374673130279658</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.6">
@@ -10462,15 +10462,15 @@
       </c>
       <c r="K93" s="1">
         <f>ROUND($J93+($E$153-$J$153),2)</f>
-        <v>-8.19</v>
+        <v>-7.89</v>
       </c>
       <c r="L93" s="1">
         <f>IF($P$7="Pre-election",ROUND($K93+($P$8-$E$153),2),ROUND($C93+($P$8-$C$153),2))</f>
-        <v>-5.46</v>
+        <v>-6.99</v>
       </c>
       <c r="M93" s="1">
         <f>_xlfn.NORM.DIST(0,$L93,3.3,TRUE)</f>
-        <v>0.95099163213844129</v>
+        <v>0.98292016380006697</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.6">
@@ -10502,15 +10502,15 @@
       </c>
       <c r="K94" s="1">
         <f>ROUND($J94+($E$153-$J$153),2)</f>
-        <v>-2.79</v>
+        <v>-2.4900000000000002</v>
       </c>
       <c r="L94" s="1">
         <f>IF($P$7="Pre-election",ROUND($K94+($P$8-$E$153),2),ROUND($C94+($P$8-$C$153),2))</f>
-        <v>3.28</v>
+        <v>1.75</v>
       </c>
       <c r="M94" s="1">
         <f>_xlfn.NORM.DIST(0,$L94,3.3,TRUE)</f>
-        <v>0.16012618705051573</v>
+        <v>0.29795092300728476</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.6">
@@ -10536,15 +10536,15 @@
       </c>
       <c r="K95" s="1">
         <f>ROUND($J95+($E$153-$J$153),2)</f>
-        <v>11.63</v>
+        <v>11.93</v>
       </c>
       <c r="L95" s="1">
         <f>IF($P$7="Pre-election",ROUND($K95+($P$8-$E$153),2),ROUND($C95+($P$8-$C$153),2))</f>
-        <v>15.17</v>
+        <v>13.64</v>
       </c>
       <c r="M95" s="1">
         <f>_xlfn.NORM.DIST(0,$L95,3.3,TRUE)</f>
-        <v>2.1433996861443319E-6</v>
+        <v>1.7876979701243996E-5</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.6">
@@ -10576,15 +10576,15 @@
       </c>
       <c r="K96" s="1">
         <f>ROUND($J96+($E$153-$J$153),2)</f>
-        <v>-5.83</v>
+        <v>-5.53</v>
       </c>
       <c r="L96" s="1">
         <f>IF($P$7="Pre-election",ROUND($K96+($P$8-$E$153),2),ROUND($C96+($P$8-$C$153),2))</f>
-        <v>-5.18</v>
+        <v>-6.71</v>
       </c>
       <c r="M96" s="1">
         <f>_xlfn.NORM.DIST(0,$L96,3.3,TRUE)</f>
-        <v>0.94175718672473108</v>
+        <v>0.9789905711601572</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.6">
@@ -10616,15 +10616,15 @@
       </c>
       <c r="K97" s="1">
         <f>ROUND($J97+($E$153-$J$153),2)</f>
-        <v>-10.33</v>
+        <v>-10.029999999999999</v>
       </c>
       <c r="L97" s="1">
         <f>IF($P$7="Pre-election",ROUND($K97+($P$8-$E$153),2),ROUND($C97+($P$8-$C$153),2))</f>
-        <v>-8.4</v>
+        <v>-9.93</v>
       </c>
       <c r="M97" s="1">
         <f>_xlfn.NORM.DIST(0,$L97,3.3,TRUE)</f>
-        <v>0.99454322142594231</v>
+        <v>0.99868984651367576</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.6">
@@ -10650,15 +10650,15 @@
       </c>
       <c r="K98" s="1">
         <f>ROUND($J98+($E$153-$J$153),2)</f>
-        <v>15.74</v>
+        <v>16.04</v>
       </c>
       <c r="L98" s="1">
         <f>IF($P$7="Pre-election",ROUND($K98+($P$8-$E$153),2),ROUND($C98+($P$8-$C$153),2))</f>
-        <v>13.22</v>
+        <v>11.69</v>
       </c>
       <c r="M98" s="1">
         <f>_xlfn.NORM.DIST(0,$L98,3.3,TRUE)</f>
-        <v>3.0869906886562556E-5</v>
+        <v>1.9823364221020258E-4</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.6">
@@ -10687,15 +10687,15 @@
       </c>
       <c r="K99" s="1">
         <f>ROUND($J99+($E$153-$J$153),2)</f>
-        <v>-0.21</v>
+        <v>0.09</v>
       </c>
       <c r="L99" s="1">
         <f>IF($P$7="Pre-election",ROUND($K99+($P$8-$E$153),2),ROUND($C99+($P$8-$C$153),2))</f>
-        <v>-6.25</v>
+        <v>-7.78</v>
       </c>
       <c r="M99" s="1">
         <f>_xlfn.NORM.DIST(0,$L99,3.3,TRUE)</f>
-        <v>0.97088347259668106</v>
+        <v>0.9908026492209423</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.6">
@@ -10727,15 +10727,15 @@
       </c>
       <c r="K100" s="1">
         <f>ROUND($J100+($E$153-$J$153),2)</f>
-        <v>-4.1900000000000004</v>
+        <v>-3.89</v>
       </c>
       <c r="L100" s="1">
         <f>IF($P$7="Pre-election",ROUND($K100+($P$8-$E$153),2),ROUND($C100+($P$8-$C$153),2))</f>
-        <v>-0.19</v>
+        <v>-1.72</v>
       </c>
       <c r="M100" s="1">
         <f>_xlfn.NORM.DIST(0,$L100,3.3,TRUE)</f>
-        <v>0.52295671985821479</v>
+        <v>0.69889049441981066</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.6">
@@ -10761,15 +10761,15 @@
       </c>
       <c r="K101" s="1">
         <f>ROUND($J101+($E$153-$J$153),2)</f>
-        <v>-10.79</v>
+        <v>-10.49</v>
       </c>
       <c r="L101" s="1">
         <f>IF($P$7="Pre-election",ROUND($K101+($P$8-$E$153),2),ROUND($C101+($P$8-$C$153),2))</f>
-        <v>-9.7200000000000006</v>
+        <v>-11.25</v>
       </c>
       <c r="M101" s="1">
         <f>_xlfn.NORM.DIST(0,$L101,3.3,TRUE)</f>
-        <v>0.99838759736748028</v>
+        <v>0.99967410122427991</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.6">
@@ -10798,15 +10798,15 @@
       </c>
       <c r="K102" s="1">
         <f>ROUND($J102+($E$153-$J$153),2)</f>
-        <v>18.8</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="L102" s="1">
         <f>IF($P$7="Pre-election",ROUND($K102+($P$8-$E$153),2),ROUND($C102+($P$8-$C$153),2))</f>
-        <v>16.23</v>
+        <v>14.7</v>
       </c>
       <c r="M102" s="1">
         <f>_xlfn.NORM.DIST(0,$L102,3.3,TRUE)</f>
-        <v>4.3675879946044561E-7</v>
+        <v>4.203555853963149E-6</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.6">
@@ -10832,15 +10832,15 @@
       </c>
       <c r="K103" s="1">
         <f>ROUND($J103+($E$153-$J$153),2)</f>
-        <v>17.54</v>
+        <v>17.84</v>
       </c>
       <c r="L103" s="1">
         <f>IF($P$7="Pre-election",ROUND($K103+($P$8-$E$153),2),ROUND($C103+($P$8-$C$153),2))</f>
-        <v>25.42</v>
+        <v>23.89</v>
       </c>
       <c r="M103" s="1">
         <f>_xlfn.NORM.DIST(0,$L103,3.3,TRUE)</f>
-        <v>6.643841673716173E-15</v>
+        <v>2.253470837641355E-13</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.6">
@@ -10866,15 +10866,15 @@
       </c>
       <c r="K104" s="1">
         <f>ROUND($J104+($E$153-$J$153),2)</f>
-        <v>-10.4</v>
+        <v>-10.1</v>
       </c>
       <c r="L104" s="1">
         <f>IF($P$7="Pre-election",ROUND($K104+($P$8-$E$153),2),ROUND($C104+($P$8-$C$153),2))</f>
-        <v>-11.2</v>
+        <v>-12.73</v>
       </c>
       <c r="M104" s="1">
         <f>_xlfn.NORM.DIST(0,$L104,3.3,TRUE)</f>
-        <v>0.99965552531158319</v>
+        <v>0.99994274140450556</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.6">
@@ -10906,15 +10906,15 @@
       </c>
       <c r="K105" s="1">
         <f>ROUND($J105+($E$153-$J$153),2)</f>
-        <v>3.27</v>
+        <v>3.57</v>
       </c>
       <c r="L105" s="1">
         <f>IF($P$7="Pre-election",ROUND($K105+($P$8-$E$153),2),ROUND($C105+($P$8-$C$153),2))</f>
-        <v>2.54</v>
+        <v>1.01</v>
       </c>
       <c r="M105" s="1">
         <f>_xlfn.NORM.DIST(0,$L105,3.3,TRUE)</f>
-        <v>0.2207398340262455</v>
+        <v>0.37977925067343921</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.6">
@@ -10940,15 +10940,15 @@
       </c>
       <c r="K106" s="1">
         <f>ROUND($J106+($E$153-$J$153),2)</f>
-        <v>-6</v>
+        <v>-5.7</v>
       </c>
       <c r="L106" s="1">
         <f>IF($P$7="Pre-election",ROUND($K106+($P$8-$E$153),2),ROUND($C106+($P$8-$C$153),2))</f>
-        <v>-5.0199999999999996</v>
+        <v>-6.55</v>
       </c>
       <c r="M106" s="1">
         <f>_xlfn.NORM.DIST(0,$L106,3.3,TRUE)</f>
-        <v>0.9358966926820772</v>
+        <v>0.97641933435029504</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.6">
@@ -10974,15 +10974,15 @@
       </c>
       <c r="K107" s="1">
         <f>ROUND($J107+($E$153-$J$153),2)</f>
-        <v>-12.11</v>
+        <v>-11.81</v>
       </c>
       <c r="L107" s="1">
         <f>IF($P$7="Pre-election",ROUND($K107+($P$8-$E$153),2),ROUND($C107+($P$8-$C$153),2))</f>
-        <v>-6.64</v>
+        <v>-8.17</v>
       </c>
       <c r="M107" s="1">
         <f>_xlfn.NORM.DIST(0,$L107,3.3,TRUE)</f>
-        <v>0.97789641943088856</v>
+        <v>0.99335230898892291</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.6">
@@ -11008,15 +11008,15 @@
       </c>
       <c r="K108" s="1">
         <f>ROUND($J108+($E$153-$J$153),2)</f>
-        <v>11.64</v>
+        <v>11.94</v>
       </c>
       <c r="L108" s="1">
         <f>IF($P$7="Pre-election",ROUND($K108+($P$8-$E$153),2),ROUND($C108+($P$8-$C$153),2))</f>
-        <v>12.2</v>
+        <v>10.67</v>
       </c>
       <c r="M108" s="1">
         <f>_xlfn.NORM.DIST(0,$L108,3.3,TRUE)</f>
-        <v>1.0909418767093044E-4</v>
+        <v>6.1177353248620424E-4</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.6">
@@ -11048,15 +11048,15 @@
       </c>
       <c r="K109" s="1">
         <f>ROUND($J109+($E$153-$J$153),2)</f>
-        <v>-17</v>
+        <v>-16.7</v>
       </c>
       <c r="L109" s="1">
         <f>IF($P$7="Pre-election",ROUND($K109+($P$8-$E$153),2),ROUND($C109+($P$8-$C$153),2))</f>
-        <v>-17.059999999999999</v>
+        <v>-18.59</v>
       </c>
       <c r="M109" s="1">
         <f>_xlfn.NORM.DIST(0,$L109,3.3,TRUE)</f>
-        <v>0.99999988276305696</v>
+        <v>0.99999999116203309</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.6">
@@ -11082,15 +11082,15 @@
       </c>
       <c r="K110" s="1">
         <f>ROUND($J110+($E$153-$J$153),2)</f>
-        <v>7.81</v>
+        <v>8.11</v>
       </c>
       <c r="L110" s="1">
         <f>IF($P$7="Pre-election",ROUND($K110+($P$8-$E$153),2),ROUND($C110+($P$8-$C$153),2))</f>
-        <v>7.53</v>
+        <v>6</v>
       </c>
       <c r="M110" s="1">
         <f>_xlfn.NORM.DIST(0,$L110,3.3,TRUE)</f>
-        <v>1.1250038443026637E-2</v>
+        <v>3.45181739972076E-2</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.6">
@@ -11116,15 +11116,15 @@
       </c>
       <c r="K111" s="1">
         <f>ROUND($J111+($E$153-$J$153),2)</f>
-        <v>17.82</v>
+        <v>18.12</v>
       </c>
       <c r="L111" s="1">
         <f>IF($P$7="Pre-election",ROUND($K111+($P$8-$E$153),2),ROUND($C111+($P$8-$C$153),2))</f>
-        <v>18.63</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="M111" s="1">
         <f>_xlfn.NORM.DIST(0,$L111,3.3,TRUE)</f>
-        <v>8.2372697509477144E-9</v>
+        <v>1.0986667827383695E-7</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.6">
@@ -11150,15 +11150,15 @@
       </c>
       <c r="K112" s="1">
         <f>ROUND($J112+($E$153-$J$153),2)</f>
-        <v>7.51</v>
+        <v>7.81</v>
       </c>
       <c r="L112" s="1">
         <f>IF($P$7="Pre-election",ROUND($K112+($P$8-$E$153),2),ROUND($C112+($P$8-$C$153),2))</f>
-        <v>7.36</v>
+        <v>5.83</v>
       </c>
       <c r="M112" s="1">
         <f>_xlfn.NORM.DIST(0,$L112,3.3,TRUE)</f>
-        <v>1.2863666072804331E-2</v>
+        <v>3.8642034462794954E-2</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.6">
@@ -11187,15 +11187,15 @@
       </c>
       <c r="K113" s="1">
         <f>ROUND($J113+($E$153-$J$153),2)</f>
-        <v>13.61</v>
+        <v>13.91</v>
       </c>
       <c r="L113" s="1">
         <f>IF($P$7="Pre-election",ROUND($K113+($P$8-$E$153),2),ROUND($C113+($P$8-$C$153),2))</f>
-        <v>15.36</v>
+        <v>13.83</v>
       </c>
       <c r="M113" s="1">
         <f>_xlfn.NORM.DIST(0,$L113,3.3,TRUE)</f>
-        <v>1.6234810211185019E-6</v>
+        <v>1.3891948729365288E-5</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.6">
@@ -11221,15 +11221,15 @@
       </c>
       <c r="K114" s="1">
         <f>ROUND($J114+($E$153-$J$153),2)</f>
-        <v>11.02</v>
+        <v>11.32</v>
       </c>
       <c r="L114" s="1">
         <f>IF($P$7="Pre-election",ROUND($K114+($P$8-$E$153),2),ROUND($C114+($P$8-$C$153),2))</f>
-        <v>11.65</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="M114" s="1">
         <f>_xlfn.NORM.DIST(0,$L114,3.3,TRUE)</f>
-        <v>2.0754197764910905E-4</v>
+        <v>1.0823004813931914E-3</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.6">
@@ -11255,15 +11255,15 @@
       </c>
       <c r="K115" s="1">
         <f>ROUND($J115+($E$153-$J$153),2)</f>
-        <v>-4.0199999999999996</v>
+        <v>-3.72</v>
       </c>
       <c r="L115" s="1">
         <f>IF($P$7="Pre-election",ROUND($K115+($P$8-$E$153),2),ROUND($C115+($P$8-$C$153),2))</f>
-        <v>-1.9</v>
+        <v>-3.43</v>
       </c>
       <c r="M115" s="1">
         <f>_xlfn.NORM.DIST(0,$L115,3.3,TRUE)</f>
-        <v>0.71761047368847575</v>
+        <v>0.85068921923589591</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.6">
@@ -11289,15 +11289,15 @@
       </c>
       <c r="K116" s="1">
         <f>ROUND($J116+($E$153-$J$153),2)</f>
-        <v>16.420000000000002</v>
+        <v>16.72</v>
       </c>
       <c r="L116" s="1">
         <f>IF($P$7="Pre-election",ROUND($K116+($P$8-$E$153),2),ROUND($C116+($P$8-$C$153),2))</f>
-        <v>17.63</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="M116" s="1">
         <f>_xlfn.NORM.DIST(0,$L116,3.3,TRUE)</f>
-        <v>4.5855852137583035E-8</v>
+        <v>5.3369891758487271E-7</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.6">
@@ -11323,15 +11323,15 @@
       </c>
       <c r="K117" s="1">
         <f>ROUND($J117+($E$153-$J$153),2)</f>
-        <v>-13.84</v>
+        <v>-13.54</v>
       </c>
       <c r="L117" s="1">
         <f>IF($P$7="Pre-election",ROUND($K117+($P$8-$E$153),2),ROUND($C117+($P$8-$C$153),2))</f>
-        <v>-13.83</v>
+        <v>-15.36</v>
       </c>
       <c r="M117" s="1">
         <f>_xlfn.NORM.DIST(0,$L117,3.3,TRUE)</f>
-        <v>0.99998610805127064</v>
+        <v>0.99999837651897883</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.6">
@@ -11357,15 +11357,15 @@
       </c>
       <c r="K118" s="1">
         <f>ROUND($J118+($E$153-$J$153),2)</f>
-        <v>22.52</v>
+        <v>22.82</v>
       </c>
       <c r="L118" s="1">
         <f>IF($P$7="Pre-election",ROUND($K118+($P$8-$E$153),2),ROUND($C118+($P$8-$C$153),2))</f>
-        <v>20.03</v>
+        <v>18.5</v>
       </c>
       <c r="M118" s="1">
         <f>_xlfn.NORM.DIST(0,$L118,3.3,TRUE)</f>
-        <v>6.407591396532443E-10</v>
+        <v>1.0349175510157652E-8</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.6">
@@ -11391,15 +11391,15 @@
       </c>
       <c r="K119" s="1">
         <f>ROUND($J119+($E$153-$J$153),2)</f>
-        <v>13.61</v>
+        <v>13.91</v>
       </c>
       <c r="L119" s="1">
         <f>IF($P$7="Pre-election",ROUND($K119+($P$8-$E$153),2),ROUND($C119+($P$8-$C$153),2))</f>
-        <v>9.27</v>
+        <v>7.74</v>
       </c>
       <c r="M119" s="1">
         <f>_xlfn.NORM.DIST(0,$L119,3.3,TRUE)</f>
-        <v>2.4840807679279548E-3</v>
+        <v>9.5019478141671627E-3</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.6">
@@ -11425,15 +11425,15 @@
       </c>
       <c r="K120" s="1">
         <f>ROUND($J120+($E$153-$J$153),2)</f>
-        <v>15.04</v>
+        <v>15.34</v>
       </c>
       <c r="L120" s="1">
         <f>IF($P$7="Pre-election",ROUND($K120+($P$8-$E$153),2),ROUND($C120+($P$8-$C$153),2))</f>
-        <v>14.48</v>
+        <v>12.95</v>
       </c>
       <c r="M120" s="1">
         <f>_xlfn.NORM.DIST(0,$L120,3.3,TRUE)</f>
-        <v>5.7230766601282831E-6</v>
+        <v>4.3501545204933469E-5</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.6">
@@ -11459,15 +11459,15 @@
       </c>
       <c r="K121" s="1">
         <f>ROUND($J121+($E$153-$J$153),2)</f>
-        <v>-9.02</v>
+        <v>-8.7200000000000006</v>
       </c>
       <c r="L121" s="1">
         <f>IF($P$7="Pre-election",ROUND($K121+($P$8-$E$153),2),ROUND($C121+($P$8-$C$153),2))</f>
-        <v>-6.4</v>
+        <v>-7.93</v>
       </c>
       <c r="M121" s="1">
         <f>_xlfn.NORM.DIST(0,$L121,3.3,TRUE)</f>
-        <v>0.9737733060281597</v>
+        <v>0.99187008001058796</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.6">
@@ -11493,15 +11493,15 @@
       </c>
       <c r="K122" s="1">
         <f>ROUND($J122+($E$153-$J$153),2)</f>
-        <v>2.2999999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="L122" s="1">
         <f>IF($P$7="Pre-election",ROUND($K122+($P$8-$E$153),2),ROUND($C122+($P$8-$C$153),2))</f>
-        <v>9.4499999999999993</v>
+        <v>7.92</v>
       </c>
       <c r="M122" s="1">
         <f>_xlfn.NORM.DIST(0,$L122,3.3,TRUE)</f>
-        <v>2.0940425067922761E-3</v>
+        <v>8.1975359245961311E-3</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.6">
@@ -11527,15 +11527,15 @@
       </c>
       <c r="K123" s="1">
         <f>ROUND($J123+($E$153-$J$153),2)</f>
-        <v>15.1</v>
+        <v>15.4</v>
       </c>
       <c r="L123" s="1">
         <f>IF($P$7="Pre-election",ROUND($K123+($P$8-$E$153),2),ROUND($C123+($P$8-$C$153),2))</f>
-        <v>16.91</v>
+        <v>15.38</v>
       </c>
       <c r="M123" s="1">
         <f>_xlfn.NORM.DIST(0,$L123,3.3,TRUE)</f>
-        <v>1.4936821069307964E-7</v>
+        <v>1.5763982316326723E-6</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.6">
@@ -11561,15 +11561,15 @@
       </c>
       <c r="K124" s="1">
         <f>ROUND($J124+($E$153-$J$153),2)</f>
-        <v>-7.67</v>
+        <v>-7.37</v>
       </c>
       <c r="L124" s="1">
         <f>IF($P$7="Pre-election",ROUND($K124+($P$8-$E$153),2),ROUND($C124+($P$8-$C$153),2))</f>
-        <v>-3.5</v>
+        <v>-5.03</v>
       </c>
       <c r="M124" s="1">
         <f>_xlfn.NORM.DIST(0,$L124,3.3,TRUE)</f>
-        <v>0.85556551643801737</v>
+        <v>0.93627591806313015</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.6">
@@ -11601,15 +11601,15 @@
       </c>
       <c r="K125" s="1">
         <f>ROUND($J125+($E$153-$J$153),2)</f>
-        <v>-12.74</v>
+        <v>-12.44</v>
       </c>
       <c r="L125" s="1">
         <f>IF($P$7="Pre-election",ROUND($K125+($P$8-$E$153),2),ROUND($C125+($P$8-$C$153),2))</f>
-        <v>-5.04</v>
+        <v>-6.57</v>
       </c>
       <c r="M125" s="1">
         <f>_xlfn.NORM.DIST(0,$L125,3.3,TRUE)</f>
-        <v>0.93665339587422114</v>
+        <v>0.97675455870747474</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.6">
@@ -11635,15 +11635,15 @@
       </c>
       <c r="K126" s="1">
         <f>ROUND($J126+($E$153-$J$153),2)</f>
-        <v>3.63</v>
+        <v>3.93</v>
       </c>
       <c r="L126" s="1">
         <f>IF($P$7="Pre-election",ROUND($K126+($P$8-$E$153),2),ROUND($C126+($P$8-$C$153),2))</f>
-        <v>7.52</v>
+        <v>5.99</v>
       </c>
       <c r="M126" s="1">
         <f>_xlfn.NORM.DIST(0,$L126,3.3,TRUE)</f>
-        <v>1.1339838896237648E-2</v>
+        <v>3.475031416518131E-2</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.6">
@@ -11669,15 +11669,15 @@
       </c>
       <c r="K127" s="1">
         <f>ROUND($J127+($E$153-$J$153),2)</f>
-        <v>-3.33</v>
+        <v>-3.03</v>
       </c>
       <c r="L127" s="1">
         <f>IF($P$7="Pre-election",ROUND($K127+($P$8-$E$153),2),ROUND($C127+($P$8-$C$153),2))</f>
-        <v>-4.93</v>
+        <v>-6.46</v>
       </c>
       <c r="M127" s="1">
         <f>_xlfn.NORM.DIST(0,$L127,3.3,TRUE)</f>
-        <v>0.93240426962959433</v>
+        <v>0.97486009285525377</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.6">
@@ -11703,15 +11703,15 @@
       </c>
       <c r="K128" s="1">
         <f>ROUND($J128+($E$153-$J$153),2)</f>
-        <v>1.65</v>
+        <v>1.95</v>
       </c>
       <c r="L128" s="1">
         <f>IF($P$7="Pre-election",ROUND($K128+($P$8-$E$153),2),ROUND($C128+($P$8-$C$153),2))</f>
-        <v>8.4</v>
+        <v>6.87</v>
       </c>
       <c r="M128" s="1">
         <f>_xlfn.NORM.DIST(0,$L128,3.3,TRUE)</f>
-        <v>5.4567785740577248E-3</v>
+        <v>1.8679540178275635E-2</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.6">
@@ -11737,15 +11737,15 @@
       </c>
       <c r="K129" s="1">
         <f>ROUND($J129+($E$153-$J$153),2)</f>
-        <v>-11.3</v>
+        <v>-11</v>
       </c>
       <c r="L129" s="1">
         <f>IF($P$7="Pre-election",ROUND($K129+($P$8-$E$153),2),ROUND($C129+($P$8-$C$153),2))</f>
-        <v>-6.44</v>
+        <v>-7.97</v>
       </c>
       <c r="M129" s="1">
         <f>_xlfn.NORM.DIST(0,$L129,3.3,TRUE)</f>
-        <v>0.97450210219400268</v>
+        <v>0.9921356673196724</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.6">
@@ -11774,15 +11774,15 @@
       </c>
       <c r="K130" s="1">
         <f>ROUND($J130+($E$153-$J$153),2)</f>
-        <v>3.69</v>
+        <v>3.99</v>
       </c>
       <c r="L130" s="1">
         <f>IF($P$7="Pre-election",ROUND($K130+($P$8-$E$153),2),ROUND($C130+($P$8-$C$153),2))</f>
-        <v>3.18</v>
+        <v>1.65</v>
       </c>
       <c r="M130" s="1">
         <f>_xlfn.NORM.DIST(0,$L130,3.3,TRUE)</f>
-        <v>0.16761413450369333</v>
+        <v>0.30853753872598688</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.6">
@@ -11808,15 +11808,15 @@
       </c>
       <c r="K131" s="1">
         <f>ROUND($J131+($E$153-$J$153),2)</f>
-        <v>-3.96</v>
+        <v>-3.66</v>
       </c>
       <c r="L131" s="1">
         <f>IF($P$7="Pre-election",ROUND($K131+($P$8-$E$153),2),ROUND($C131+($P$8-$C$153),2))</f>
-        <v>-4.08</v>
+        <v>-5.61</v>
       </c>
       <c r="M131" s="1">
         <f>_xlfn.NORM.DIST(0,$L131,3.3,TRUE)</f>
-        <v>0.89183828674756216</v>
+        <v>0.95543453724145699</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.6">
@@ -11842,15 +11842,15 @@
       </c>
       <c r="K132" s="1">
         <f>ROUND($J132+($E$153-$J$153),2)</f>
-        <v>16.440000000000001</v>
+        <v>16.739999999999998</v>
       </c>
       <c r="L132" s="1">
         <f>IF($P$7="Pre-election",ROUND($K132+($P$8-$E$153),2),ROUND($C132+($P$8-$C$153),2))</f>
-        <v>19.48</v>
+        <v>17.95</v>
       </c>
       <c r="M132" s="1">
         <f>_xlfn.NORM.DIST(0,$L132,3.3,TRUE)</f>
-        <v>1.7844234479708914E-9</v>
+        <v>2.6731062150888162E-8</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.6">
@@ -11876,15 +11876,15 @@
       </c>
       <c r="K133" s="1">
         <f>ROUND($J133+($E$153-$J$153),2)</f>
-        <v>1.1399999999999999</v>
+        <v>1.44</v>
       </c>
       <c r="L133" s="1">
         <f>IF($P$7="Pre-election",ROUND($K133+($P$8-$E$153),2),ROUND($C133+($P$8-$C$153),2))</f>
-        <v>4.24</v>
+        <v>2.71</v>
       </c>
       <c r="M133" s="1">
         <f>_xlfn.NORM.DIST(0,$L133,3.3,TRUE)</f>
-        <v>9.9422617837206656E-2</v>
+        <v>0.20576272669947254</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.6">
@@ -11913,15 +11913,15 @@
       </c>
       <c r="K134" s="1">
         <f>ROUND($J134+($E$153-$J$153),2)</f>
-        <v>7.98</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="L134" s="1">
         <f>IF($P$7="Pre-election",ROUND($K134+($P$8-$E$153),2),ROUND($C134+($P$8-$C$153),2))</f>
-        <v>6.03</v>
+        <v>4.5</v>
       </c>
       <c r="M134" s="1">
         <f>_xlfn.NORM.DIST(0,$L134,3.3,TRUE)</f>
-        <v>3.3829386844964837E-2</v>
+        <v>8.6341020709374147E-2</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.6">
@@ -11947,15 +11947,15 @@
       </c>
       <c r="K135" s="1">
         <f>ROUND($J135+($E$153-$J$153),2)</f>
-        <v>-19.579999999999998</v>
+        <v>-19.28</v>
       </c>
       <c r="L135" s="1">
         <f>IF($P$7="Pre-election",ROUND($K135+($P$8-$E$153),2),ROUND($C135+($P$8-$C$153),2))</f>
-        <v>-21.66</v>
+        <v>-23.19</v>
       </c>
       <c r="M135" s="1">
         <f>_xlfn.NORM.DIST(0,$L135,3.3,TRUE)</f>
-        <v>0.99999999997374445</v>
+        <v>0.99999999999894695</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.6">
@@ -11981,15 +11981,15 @@
       </c>
       <c r="K136" s="1">
         <f>ROUND($J136+($E$153-$J$153),2)</f>
-        <v>-9.94</v>
+        <v>-9.64</v>
       </c>
       <c r="L136" s="1">
         <f>IF($P$7="Pre-election",ROUND($K136+($P$8-$E$153),2),ROUND($C136+($P$8-$C$153),2))</f>
-        <v>-4.45</v>
+        <v>-5.98</v>
       </c>
       <c r="M136" s="1">
         <f>_xlfn.NORM.DIST(0,$L136,3.3,TRUE)</f>
-        <v>0.91124875491686996</v>
+        <v>0.96501626527216577</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.6">
@@ -12021,15 +12021,15 @@
       </c>
       <c r="K137" s="1">
         <f>ROUND($J137+($E$153-$J$153),2)</f>
-        <v>-8.09</v>
+        <v>-7.79</v>
       </c>
       <c r="L137" s="1">
         <f>IF($P$7="Pre-election",ROUND($K137+($P$8-$E$153),2),ROUND($C137+($P$8-$C$153),2))</f>
-        <v>-3.08</v>
+        <v>-4.6100000000000003</v>
       </c>
       <c r="M137" s="1">
         <f>_xlfn.NORM.DIST(0,$L137,3.3,TRUE)</f>
-        <v>0.82467605514777054</v>
+        <v>0.91878865807203902</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.6">
@@ -12055,15 +12055,15 @@
       </c>
       <c r="K138" s="1">
         <f>ROUND($J138+($E$153-$J$153),2)</f>
-        <v>-17.170000000000002</v>
+        <v>-16.87</v>
       </c>
       <c r="L138" s="1">
         <f>IF($P$7="Pre-election",ROUND($K138+($P$8-$E$153),2),ROUND($C138+($P$8-$C$153),2))</f>
-        <v>-14.13</v>
+        <v>-15.66</v>
       </c>
       <c r="M138" s="1">
         <f>_xlfn.NORM.DIST(0,$L138,3.3,TRUE)</f>
-        <v>0.99999073137893579</v>
+        <v>0.99999895980685571</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.6">
@@ -12092,15 +12092,15 @@
       </c>
       <c r="K139" s="1">
         <f>ROUND($J139+($E$153-$J$153),2)</f>
-        <v>5.12</v>
+        <v>5.42</v>
       </c>
       <c r="L139" s="1">
         <f>IF($P$7="Pre-election",ROUND($K139+($P$8-$E$153),2),ROUND($C139+($P$8-$C$153),2))</f>
-        <v>5.65</v>
+        <v>4.12</v>
       </c>
       <c r="M139" s="1">
         <f>_xlfn.NORM.DIST(0,$L139,3.3,TRUE)</f>
-        <v>4.3437166506769313E-2</v>
+        <v>0.10592677683018896</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.6">
@@ -12129,15 +12129,15 @@
       </c>
       <c r="K140" s="1">
         <f>ROUND($J140+($E$153-$J$153),2)</f>
-        <v>4.3899999999999997</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="L140" s="1">
         <f>IF($P$7="Pre-election",ROUND($K140+($P$8-$E$153),2),ROUND($C140+($P$8-$C$153),2))</f>
-        <v>6.87</v>
+        <v>5.34</v>
       </c>
       <c r="M140" s="1">
         <f>_xlfn.NORM.DIST(0,$L140,3.3,TRUE)</f>
-        <v>1.8679540178275635E-2</v>
+        <v>5.2811710001670391E-2</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.6">
@@ -12163,15 +12163,15 @@
       </c>
       <c r="K141" s="1">
         <f>ROUND($J141+($E$153-$J$153),2)</f>
-        <v>3.59</v>
+        <v>3.89</v>
       </c>
       <c r="L141" s="1">
         <f>IF($P$7="Pre-election",ROUND($K141+($P$8-$E$153),2),ROUND($C141+($P$8-$C$153),2))</f>
-        <v>2.69</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="M141" s="1">
         <f>_xlfn.NORM.DIST(0,$L141,3.3,TRUE)</f>
-        <v>0.20749279350234062</v>
+        <v>0.36260095378583457</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.6">
@@ -12197,15 +12197,15 @@
       </c>
       <c r="K142" s="1">
         <f>ROUND($J142+($E$153-$J$153),2)</f>
-        <v>-15.31</v>
+        <v>-15.01</v>
       </c>
       <c r="L142" s="1">
         <f>IF($P$7="Pre-election",ROUND($K142+($P$8-$E$153),2),ROUND($C142+($P$8-$C$153),2))</f>
-        <v>-18.670000000000002</v>
+        <v>-20.2</v>
       </c>
       <c r="M142" s="1">
         <f>_xlfn.NORM.DIST(0,$L142,3.3,TRUE)</f>
-        <v>0.99999999232369718</v>
+        <v>0.99999999953566909</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.6">
@@ -12231,15 +12231,15 @@
       </c>
       <c r="K143" s="1">
         <f>ROUND($J143+($E$153-$J$153),2)</f>
-        <v>11.07</v>
+        <v>11.37</v>
       </c>
       <c r="L143" s="1">
         <f>IF($P$7="Pre-election",ROUND($K143+($P$8-$E$153),2),ROUND($C143+($P$8-$C$153),2))</f>
-        <v>11.47</v>
+        <v>9.94</v>
       </c>
       <c r="M143" s="1">
         <f>_xlfn.NORM.DIST(0,$L143,3.3,TRUE)</f>
-        <v>2.5470627186878773E-4</v>
+        <v>1.2971449207668877E-3</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.6">
@@ -12265,15 +12265,15 @@
       </c>
       <c r="K144" s="1">
         <f>ROUND($J144+($E$153-$J$153),2)</f>
-        <v>9.16</v>
+        <v>9.4600000000000009</v>
       </c>
       <c r="L144" s="1">
         <f>IF($P$7="Pre-election",ROUND($K144+($P$8-$E$153),2),ROUND($C144+($P$8-$C$153),2))</f>
-        <v>10.39</v>
+        <v>8.86</v>
       </c>
       <c r="M144" s="1">
         <f>_xlfn.NORM.DIST(0,$L144,3.3,TRUE)</f>
-        <v>8.2059615537345817E-4</v>
+        <v>3.6281346484320302E-3</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.6">
@@ -12302,15 +12302,15 @@
       </c>
       <c r="K145" s="1">
         <f>ROUND($J145+($E$153-$J$153),2)</f>
-        <v>11.09</v>
+        <v>11.39</v>
       </c>
       <c r="L145" s="1">
         <f>IF($P$7="Pre-election",ROUND($K145+($P$8-$E$153),2),ROUND($C145+($P$8-$C$153),2))</f>
-        <v>2.12</v>
+        <v>0.59</v>
       </c>
       <c r="M145" s="1">
         <f>_xlfn.NORM.DIST(0,$L145,3.3,TRUE)</f>
-        <v>0.260298881736718</v>
+        <v>0.42905213162845096</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.6">
@@ -12336,15 +12336,15 @@
       </c>
       <c r="K146" s="1">
         <f>ROUND($J146+($E$153-$J$153),2)</f>
-        <v>-17.579999999999998</v>
+        <v>-17.28</v>
       </c>
       <c r="L146" s="1">
         <f>IF($P$7="Pre-election",ROUND($K146+($P$8-$E$153),2),ROUND($C146+($P$8-$C$153),2))</f>
-        <v>-13.52</v>
+        <v>-15.05</v>
       </c>
       <c r="M146" s="1">
         <f>_xlfn.NORM.DIST(0,$L146,3.3,TRUE)</f>
-        <v>0.9999790703163387</v>
+        <v>0.99999744969041604</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.6">
@@ -12373,15 +12373,15 @@
       </c>
       <c r="K147" s="1">
         <f>ROUND($J147+($E$153-$J$153),2)</f>
-        <v>17.75</v>
+        <v>18.05</v>
       </c>
       <c r="L147" s="1">
         <f>IF($P$7="Pre-election",ROUND($K147+($P$8-$E$153),2),ROUND($C147+($P$8-$C$153),2))</f>
-        <v>9.85</v>
+        <v>8.32</v>
       </c>
       <c r="M147" s="1">
         <f>_xlfn.NORM.DIST(0,$L147,3.3,TRUE)</f>
-        <v>1.4185940984381463E-3</v>
+        <v>5.8475663663904894E-3</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.6">
@@ -12407,15 +12407,15 @@
       </c>
       <c r="K148" s="1">
         <f>ROUND($J148+($E$153-$J$153),2)</f>
-        <v>-8.1999999999999993</v>
+        <v>-7.9</v>
       </c>
       <c r="L148" s="1">
         <f>IF($P$7="Pre-election",ROUND($K148+($P$8-$E$153),2),ROUND($C148+($P$8-$C$153),2))</f>
-        <v>-5.47</v>
+        <v>-7</v>
       </c>
       <c r="M148" s="1">
         <f>_xlfn.NORM.DIST(0,$L148,3.3,TRUE)</f>
-        <v>0.95129843692518801</v>
+        <v>0.98304802215960851</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.6">
@@ -12441,15 +12441,15 @@
       </c>
       <c r="K149" s="1">
         <f>ROUND($J149+($E$153-$J$153),2)</f>
-        <v>-13.72</v>
+        <v>-13.42</v>
       </c>
       <c r="L149" s="1">
         <f>IF($P$7="Pre-election",ROUND($K149+($P$8-$E$153),2),ROUND($C149+($P$8-$C$153),2))</f>
-        <v>-10.91</v>
+        <v>-12.44</v>
       </c>
       <c r="M149" s="1">
         <f>_xlfn.NORM.DIST(0,$L149,3.3,TRUE)</f>
-        <v>0.99952691190081266</v>
+        <v>0.99991827706271752</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.6">
@@ -12475,15 +12475,15 @@
       </c>
       <c r="K150" s="1">
         <f>ROUND($J150+($E$153-$J$153),2)</f>
-        <v>8.19</v>
+        <v>8.49</v>
       </c>
       <c r="L150" s="1">
         <f>IF($P$7="Pre-election",ROUND($K150+($P$8-$E$153),2),ROUND($C150+($P$8-$C$153),2))</f>
-        <v>13.15</v>
+        <v>11.62</v>
       </c>
       <c r="M150" s="1">
         <f>_xlfn.NORM.DIST(0,$L150,3.3,TRUE)</f>
-        <v>3.3761598096283407E-5</v>
+        <v>2.1478941385689662E-4</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.6">
@@ -12509,15 +12509,15 @@
       </c>
       <c r="K151" s="1">
         <f>ROUND($J151+($E$153-$J$153),2)</f>
-        <v>-21.67</v>
+        <v>-21.37</v>
       </c>
       <c r="L151" s="1">
         <f>IF($P$7="Pre-election",ROUND($K151+($P$8-$E$153),2),ROUND($C151+($P$8-$C$153),2))</f>
-        <v>-25.85</v>
+        <v>-27.38</v>
       </c>
       <c r="M151" s="1">
         <f>_xlfn.NORM.DIST(0,$L151,3.3,TRUE)</f>
-        <v>0.99999999999999767</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.6">
@@ -12536,6 +12536,34 @@
       <c r="E152" s="1">
         <f>ROUND(C152-D152,3)</f>
         <v>9.6170000000000009</v>
+      </c>
+      <c r="J152" s="1">
+        <f>ROUND($E152+IF($I152="ALP",-1,IF(OR($I152="LIB",$I152="NAT",$I152="LIB/NAT"),1,0))-IF($H152="ALP",-1,IF(OR($H152="LIB",$H152="NAT",$H152="LIB/NAT"),1,0)),2)</f>
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="K152" s="1">
+        <f>ROUND($J152+($E$153-$J$153),2)</f>
+        <v>9.92</v>
+      </c>
+      <c r="L152" s="1">
+        <f>IF($P$7="Pre-election",ROUND($K152+($P$8-$E$153),2),ROUND($C152+($P$8-$C$153),2))</f>
+        <v>13.05</v>
+      </c>
+      <c r="M152" s="1">
+        <f>_xlfn.NORM.DIST(0,$L152,3.3,TRUE)</f>
+        <v>3.8340146648025316E-5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.6">
+      <c r="C153" s="1">
+        <v>1.53</v>
+      </c>
+      <c r="E153" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="J153" s="1">
+        <f>ROUND(SUMPRODUCT($B$2:$B152,J$2:J152)/SUM($B$2:$B152),2)</f>
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>
@@ -12560,7 +12588,9 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:R150"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>
@@ -17961,7 +17991,9 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:R150"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I149"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>
@@ -23357,7 +23389,9 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:R149"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I148"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>
@@ -28785,7 +28819,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>
@@ -34222,7 +34258,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I151"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>
@@ -39986,7 +40024,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I151"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>
@@ -46155,7 +46195,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I151"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>
@@ -52324,7 +52366,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R152"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I151"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.6"/>
   <cols>

</xml_diff>